<commit_message>
Changed env table log
</commit_message>
<xml_diff>
--- a/Reports/EnvBobLog.xlsx
+++ b/Reports/EnvBobLog.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:X52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -634,72 +634,72 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>163.951872253482</v>
+        <v>163.9731205251298</v>
       </c>
       <c r="D3" t="n">
-        <v>1.119161105026625</v>
+        <v>1.055284896272224</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:21.000000000</t>
+          <t>22 Jun 2025 10:15:20.000000000</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>-1.017690395454713</v>
+        <v>97.24842937034347</v>
       </c>
       <c r="G3" t="n">
-        <v>-4.027990352094526</v>
+        <v>94.23812941370366</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1868839761532532</v>
+        <v>1e-30</v>
       </c>
       <c r="I3" t="n">
-        <v>2808.932536949855</v>
+        <v>2815.78946910655</v>
       </c>
       <c r="J3" t="n">
-        <v>-2.091192473021252</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K3" t="n">
-        <v>187.5256367855042</v>
+        <v>187.5468142180631</v>
       </c>
       <c r="L3" t="n">
-        <v>64.81132512317259</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>-90.46397664504035</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>-32.09119247302125</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O3" t="n">
         <v>30</v>
       </c>
       <c r="P3" t="n">
-        <v>-189.6168292585255</v>
+        <v>-91.35070949272732</v>
       </c>
       <c r="Q3" t="n">
-        <v>-189.6168292585255</v>
+        <v>-91.35070949272732</v>
       </c>
       <c r="R3" t="n">
-        <v>4070.988386033326</v>
+        <v>4064.853260246761</v>
       </c>
       <c r="S3" t="n">
-        <v>783.022232764853</v>
+        <v>783.622530847562</v>
       </c>
       <c r="T3" t="n">
-        <v>-5648.674176296665</v>
+        <v>-5653.008471228448</v>
       </c>
       <c r="U3" t="n">
-        <v>6.132905450005919</v>
+        <v>6.137604883762061</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.6007518145096375</v>
+        <v>-0.5998468732038993</v>
       </c>
       <c r="W3" t="n">
-        <v>4.337652218543272</v>
+        <v>4.331106433195484</v>
       </c>
       <c r="X3" t="n">
-        <v>7.535825022542807</v>
+        <v>7.535814018149579</v>
       </c>
     </row>
     <row r="4">
@@ -710,72 +710,72 @@
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>163.9305370533707</v>
+        <v>163.951872253482</v>
       </c>
       <c r="D4" t="n">
-        <v>1.183197228970335</v>
+        <v>1.119161105026625</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:22.000000000</t>
+          <t>22 Jun 2025 10:15:21.000000000</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>-1.167490410837526</v>
+        <v>80.9859195163932</v>
       </c>
       <c r="G4" t="n">
-        <v>-4.177790367477338</v>
+        <v>77.97561955975338</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1909966305433188</v>
+        <v>1e-30</v>
       </c>
       <c r="I4" t="n">
-        <v>2802.075916028852</v>
+        <v>2808.932536949855</v>
       </c>
       <c r="J4" t="n">
-        <v>-2.262220716004624</v>
+        <v>79.91241743882667</v>
       </c>
       <c r="K4" t="n">
-        <v>187.5044085579037</v>
+        <v>187.5256367855042</v>
       </c>
       <c r="L4" t="n">
-        <v>64.84549280046785</v>
+        <v>0.06731639098841398</v>
       </c>
       <c r="M4" t="n">
-        <v>-90.5224101715478</v>
+        <v>-18.0931802693189</v>
       </c>
       <c r="N4" t="n">
-        <v>-32.26222071600462</v>
+        <v>49.91241743882667</v>
       </c>
       <c r="O4" t="n">
         <v>30</v>
       </c>
       <c r="P4" t="n">
-        <v>-189.7666292739083</v>
+        <v>-107.6132193466776</v>
       </c>
       <c r="Q4" t="n">
-        <v>-189.7666292739083</v>
+        <v>-107.6132193466776</v>
       </c>
       <c r="R4" t="n">
-        <v>4077.118808914962</v>
+        <v>4070.988386033326</v>
       </c>
       <c r="S4" t="n">
-        <v>782.4210301022945</v>
+        <v>783.022232764853</v>
       </c>
       <c r="T4" t="n">
-        <v>-5644.333338211622</v>
+        <v>-5648.674176296665</v>
       </c>
       <c r="U4" t="n">
-        <v>6.128198897917392</v>
+        <v>6.132905450005919</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.6016560682165223</v>
+        <v>-0.6007518145096375</v>
       </c>
       <c r="W4" t="n">
-        <v>4.344193025594505</v>
+        <v>4.337652218543272</v>
       </c>
       <c r="X4" t="n">
-        <v>7.535836038587997</v>
+        <v>7.535825022542807</v>
       </c>
     </row>
     <row r="5">
@@ -786,72 +786,72 @@
         <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>163.9091141611784</v>
+        <v>163.951872253482</v>
       </c>
       <c r="D5" t="n">
-        <v>1.247394412869366</v>
+        <v>1.119161105026625</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:23.000000000</t>
+          <t>22 Jun 2025 10:15:21.000000000</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>-3.018881556619446</v>
+        <v>97.26960680290232</v>
       </c>
       <c r="G5" t="n">
-        <v>-6.029181513259259</v>
+        <v>94.2593068462625</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2399670661191066</v>
+        <v>1e-30</v>
       </c>
       <c r="I5" t="n">
-        <v>2795.219618218265</v>
+        <v>2808.932536949855</v>
       </c>
       <c r="J5" t="n">
-        <v>-4.13489109406208</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K5" t="n">
-        <v>187.4831293256281</v>
+        <v>187.5256367855042</v>
       </c>
       <c r="L5" t="n">
-        <v>64.94583378566126</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>-90.63161745223364</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.13489109406208</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O5" t="n">
         <v>30</v>
       </c>
       <c r="P5" t="n">
-        <v>-191.6180204196902</v>
+        <v>-91.32953206016848</v>
       </c>
       <c r="Q5" t="n">
-        <v>-191.6180204196902</v>
+        <v>-91.32953206016848</v>
       </c>
       <c r="R5" t="n">
-        <v>4083.244521195483</v>
+        <v>4070.988386033326</v>
       </c>
       <c r="S5" t="n">
-        <v>781.818926537306</v>
+        <v>783.022232764853</v>
       </c>
       <c r="T5" t="n">
-        <v>-5639.985961961392</v>
+        <v>-5648.674176296665</v>
       </c>
       <c r="U5" t="n">
-        <v>6.123485233249508</v>
+        <v>6.132905450005919</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.6025596288163938</v>
+        <v>-0.6007518145096375</v>
       </c>
       <c r="W5" t="n">
-        <v>4.350728846732242</v>
+        <v>4.337652218543272</v>
       </c>
       <c r="X5" t="n">
-        <v>7.535847066248904</v>
+        <v>7.535825022542807</v>
       </c>
     </row>
     <row r="6">
@@ -862,72 +862,72 @@
         <v>9</v>
       </c>
       <c r="C6" t="n">
-        <v>163.8876029772208</v>
+        <v>163.9305370533707</v>
       </c>
       <c r="D6" t="n">
-        <v>1.311753843689574</v>
+        <v>1.183197228970335</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:24.000000000</t>
+          <t>22 Jun 2025 10:15:22.000000000</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>-12.6179991483189</v>
+        <v>80.86100485750494</v>
       </c>
       <c r="G6" t="n">
-        <v>-15.62829910495871</v>
+        <v>77.85070490086513</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4075167085987591</v>
+        <v>1e-30</v>
       </c>
       <c r="I6" t="n">
-        <v>2788.363652149048</v>
+        <v>2802.075916028852</v>
       </c>
       <c r="J6" t="n">
-        <v>-13.75533914388626</v>
+        <v>79.76627455233783</v>
       </c>
       <c r="K6" t="n">
-        <v>187.4617988675034</v>
+        <v>187.5044085579037</v>
       </c>
       <c r="L6" t="n">
-        <v>65.04638678441698</v>
+        <v>0.06749542323633345</v>
       </c>
       <c r="M6" t="n">
-        <v>-90.74128791972718</v>
+        <v>-18.10116590668696</v>
       </c>
       <c r="N6" t="n">
-        <v>-43.75533914388626</v>
+        <v>49.76627455233783</v>
       </c>
       <c r="O6" t="n">
         <v>30</v>
       </c>
       <c r="P6" t="n">
-        <v>-201.2171380113897</v>
+        <v>-107.7381340055659</v>
       </c>
       <c r="Q6" t="n">
-        <v>-201.2171380113897</v>
+        <v>-107.7381340055659</v>
       </c>
       <c r="R6" t="n">
-        <v>4089.365516921297</v>
+        <v>4077.118808914962</v>
       </c>
       <c r="S6" t="n">
-        <v>781.2159167859016</v>
+        <v>782.4210301022945</v>
       </c>
       <c r="T6" t="n">
-        <v>-5635.632052527263</v>
+        <v>-5644.333338211622</v>
       </c>
       <c r="U6" t="n">
-        <v>6.118764460425718</v>
+        <v>6.128198897917392</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.6034625041831236</v>
+        <v>-0.6016560682165223</v>
       </c>
       <c r="W6" t="n">
-        <v>4.35725967437622</v>
+        <v>4.344193025594505</v>
       </c>
       <c r="X6" t="n">
-        <v>7.535858105489311</v>
+        <v>7.535836038587997</v>
       </c>
     </row>
     <row r="7">
@@ -938,72 +938,72 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>163.8660027232646</v>
+        <v>163.9305370533707</v>
       </c>
       <c r="D7" t="n">
-        <v>1.37627668812116</v>
+        <v>1.183197228970335</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:25.000000000</t>
+          <t>22 Jun 2025 10:15:22.000000000</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>-0.7127671727499731</v>
+        <v>97.29083503050288</v>
       </c>
       <c r="G7" t="n">
-        <v>-3.723067129389785</v>
+        <v>94.28053507386306</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1784687415946879</v>
+        <v>1e-30</v>
       </c>
       <c r="I7" t="n">
-        <v>2781.50802986114</v>
+        <v>2802.075916028852</v>
       </c>
       <c r="J7" t="n">
-        <v>-1.871489064369291</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K7" t="n">
-        <v>187.4404169714515</v>
+        <v>187.5044085579037</v>
       </c>
       <c r="L7" t="n">
-        <v>65.14715133140363</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>-90.85142656573042</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>-31.87148906436929</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O7" t="n">
         <v>30</v>
       </c>
       <c r="P7" t="n">
-        <v>-189.3119060358208</v>
+        <v>-91.30830383256792</v>
       </c>
       <c r="Q7" t="n">
-        <v>-189.3119060358208</v>
+        <v>-91.30830383256792</v>
       </c>
       <c r="R7" t="n">
-        <v>4095.481788411548</v>
+        <v>4077.118808914962</v>
       </c>
       <c r="S7" t="n">
-        <v>780.6120045226403</v>
+        <v>782.4210301022945</v>
       </c>
       <c r="T7" t="n">
-        <v>-5631.27161490884</v>
+        <v>-5644.333338211622</v>
       </c>
       <c r="U7" t="n">
-        <v>6.114036585211042</v>
+        <v>6.128198897917392</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.6043646888073327</v>
+        <v>-0.6016560682165223</v>
       </c>
       <c r="W7" t="n">
-        <v>4.363785500925694</v>
+        <v>4.344193025594505</v>
       </c>
       <c r="X7" t="n">
-        <v>7.535869156272923</v>
+        <v>7.535836038587997</v>
       </c>
     </row>
     <row r="8">
@@ -1014,72 +1014,72 @@
         <v>9</v>
       </c>
       <c r="C8" t="n">
-        <v>163.844312670568</v>
+        <v>163.9091141611784</v>
       </c>
       <c r="D8" t="n">
-        <v>1.440964134184426</v>
+        <v>1.247394412869366</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:26.000000000</t>
+          <t>22 Jun 2025 10:15:23.000000000</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>-4.530227956678046</v>
+        <v>80.73306817895052</v>
       </c>
       <c r="G8" t="n">
-        <v>-7.540527913317858</v>
+        <v>77.72276822231071</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2763922592074859</v>
+        <v>1e-30</v>
       </c>
       <c r="I8" t="n">
-        <v>2774.652762393974</v>
+        <v>2795.219618218265</v>
       </c>
       <c r="J8" t="n">
-        <v>-5.710383398945082</v>
+        <v>79.61705864150788</v>
       </c>
       <c r="K8" t="n">
-        <v>187.4189834208038</v>
+        <v>187.4831293256281</v>
       </c>
       <c r="L8" t="n">
-        <v>65.24812654127656</v>
+        <v>0.06767578765525117</v>
       </c>
       <c r="M8" t="n">
-        <v>-90.96203849947599</v>
+        <v>-18.10919164157201</v>
       </c>
       <c r="N8" t="n">
-        <v>-35.71038339894508</v>
+        <v>49.61705864150788</v>
       </c>
       <c r="O8" t="n">
         <v>30</v>
       </c>
       <c r="P8" t="n">
-        <v>-193.1293668197488</v>
+        <v>-107.8660706841203</v>
       </c>
       <c r="Q8" t="n">
-        <v>-193.1293668197488</v>
+        <v>-107.8660706841203</v>
       </c>
       <c r="R8" t="n">
-        <v>4101.593328551306</v>
+        <v>4083.244521195483</v>
       </c>
       <c r="S8" t="n">
-        <v>780.0071904399598</v>
+        <v>781.818926537306</v>
       </c>
       <c r="T8" t="n">
-        <v>-5626.904654122026</v>
+        <v>-5639.985961961392</v>
       </c>
       <c r="U8" t="n">
-        <v>6.109301612947864</v>
+        <v>6.123485233249508</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.6052661816410934</v>
+        <v>-0.6025596288163938</v>
       </c>
       <c r="W8" t="n">
-        <v>4.370306318775554</v>
+        <v>4.350728846732242</v>
       </c>
       <c r="X8" t="n">
-        <v>7.535880218563409</v>
+        <v>7.535847066248904</v>
       </c>
     </row>
     <row r="9">
@@ -1090,72 +1090,72 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>163.8225320244808</v>
+        <v>163.9091141611784</v>
       </c>
       <c r="D9" t="n">
-        <v>1.505817370914539</v>
+        <v>1.247394412869366</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:27.000000000</t>
+          <t>22 Jun 2025 10:15:23.000000000</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>-8.067332900405447</v>
+        <v>97.31211426277841</v>
       </c>
       <c r="G9" t="n">
-        <v>-11.07763285704526</v>
+        <v>94.3018143061386</v>
       </c>
       <c r="H9" t="n">
-        <v>0.3464092743599312</v>
+        <v>1e-30</v>
       </c>
       <c r="I9" t="n">
-        <v>2767.797861948103</v>
+        <v>2795.219618218265</v>
       </c>
       <c r="J9" t="n">
-        <v>-9.268973762443535</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K9" t="n">
-        <v>187.3974980010327</v>
+        <v>187.4831293256281</v>
       </c>
       <c r="L9" t="n">
-        <v>65.34931161798256</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>-91.07312889198091</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>-39.26897376244354</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O9" t="n">
         <v>30</v>
       </c>
       <c r="P9" t="n">
-        <v>-196.6664717634762</v>
+        <v>-91.28702460029238</v>
       </c>
       <c r="Q9" t="n">
-        <v>-196.6664717634762</v>
+        <v>-91.28702460029238</v>
       </c>
       <c r="R9" t="n">
-        <v>4107.700129693329</v>
+        <v>4083.244521195483</v>
       </c>
       <c r="S9" t="n">
-        <v>779.4014782343635</v>
+        <v>781.818926537306</v>
       </c>
       <c r="T9" t="n">
-        <v>-5622.531175166913</v>
+        <v>-5639.985961961392</v>
       </c>
       <c r="U9" t="n">
-        <v>6.104559549405135</v>
+        <v>6.123485233249508</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.6061669771973957</v>
+        <v>-0.6025596288163938</v>
       </c>
       <c r="W9" t="n">
-        <v>4.376822120357836</v>
+        <v>4.350728846732242</v>
       </c>
       <c r="X9" t="n">
-        <v>7.535891292324466</v>
+        <v>7.535847066248904</v>
       </c>
     </row>
     <row r="10">
@@ -1166,72 +1166,72 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>163.8006601567133</v>
+        <v>163.8876029772208</v>
       </c>
       <c r="D10" t="n">
-        <v>1.570837630213995</v>
+        <v>1.311753843689574</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:28.000000000</t>
+          <t>22 Jun 2025 10:15:24.000000000</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>-0.4784080638247931</v>
+        <v>80.60201838862604</v>
       </c>
       <c r="G10" t="n">
-        <v>-3.488708020464605</v>
+        <v>77.59171843198621</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1719696029860544</v>
+        <v>1e-30</v>
       </c>
       <c r="I10" t="n">
-        <v>2760.943337502153</v>
+        <v>2788.363652149048</v>
       </c>
       <c r="J10" t="n">
-        <v>-1.701586440901564</v>
+        <v>79.46467839305866</v>
       </c>
       <c r="K10" t="n">
-        <v>187.375960485994</v>
+        <v>187.4617988675034</v>
       </c>
       <c r="L10" t="n">
-        <v>65.45070567205211</v>
+        <v>0.06785747248384709</v>
       </c>
       <c r="M10" t="n">
-        <v>-91.18470274593459</v>
+        <v>-18.11711091302345</v>
       </c>
       <c r="N10" t="n">
-        <v>-31.70158644090156</v>
+        <v>49.46467839305867</v>
       </c>
       <c r="O10" t="n">
         <v>30</v>
       </c>
       <c r="P10" t="n">
-        <v>-189.0775469268956</v>
+        <v>-107.9971204744448</v>
       </c>
       <c r="Q10" t="n">
-        <v>-189.0775469268956</v>
+        <v>-107.9971204744448</v>
       </c>
       <c r="R10" t="n">
-        <v>4113.802185896458</v>
+        <v>4089.365516921297</v>
       </c>
       <c r="S10" t="n">
-        <v>778.7948625917469</v>
+        <v>781.2159167859016</v>
       </c>
       <c r="T10" t="n">
-        <v>-5618.151183058709</v>
+        <v>-5635.632052527263</v>
       </c>
       <c r="U10" t="n">
-        <v>6.099810399038263</v>
+        <v>6.118764460425718</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.6070670833234267</v>
+        <v>-0.6034625041831236</v>
       </c>
       <c r="W10" t="n">
-        <v>4.383332898108165</v>
+        <v>4.35725967437622</v>
       </c>
       <c r="X10" t="n">
-        <v>7.535902377519727</v>
+        <v>7.535858105489311</v>
       </c>
     </row>
     <row r="11">
@@ -1242,72 +1242,72 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>163.778696257454</v>
+        <v>163.8876029772208</v>
       </c>
       <c r="D11" t="n">
-        <v>1.636026123521759</v>
+        <v>1.311753843689574</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:29.000000000</t>
+          <t>22 Jun 2025 10:15:24.000000000</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>-7.207259901459339</v>
+        <v>97.33344472090315</v>
       </c>
       <c r="G11" t="n">
-        <v>-10.21755985809915</v>
+        <v>94.32314476426333</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3313635401679698</v>
+        <v>1e-30</v>
       </c>
       <c r="I11" t="n">
-        <v>2754.089201487097</v>
+        <v>2788.363652149048</v>
       </c>
       <c r="J11" t="n">
-        <v>-8.45202810569377</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K11" t="n">
-        <v>187.3543706588364</v>
+        <v>187.4617988675034</v>
       </c>
       <c r="L11" t="n">
-        <v>65.55230796830358</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>-91.29676533807658</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>-38.45202810569377</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O11" t="n">
         <v>30</v>
       </c>
       <c r="P11" t="n">
-        <v>-195.8063987645301</v>
+        <v>-91.26569414216766</v>
       </c>
       <c r="Q11" t="n">
-        <v>-195.8063987645301</v>
+        <v>-91.26569414216766</v>
       </c>
       <c r="R11" t="n">
-        <v>4119.899489477398</v>
+        <v>4089.365516921297</v>
       </c>
       <c r="S11" t="n">
-        <v>778.1873472104074</v>
+        <v>781.2159167859016</v>
       </c>
       <c r="T11" t="n">
-        <v>-5613.764682845886</v>
+        <v>-5635.632052527263</v>
       </c>
       <c r="U11" t="n">
-        <v>6.095054167668101</v>
+        <v>6.118764460425718</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.6079664945240202</v>
+        <v>-0.6034625041831236</v>
       </c>
       <c r="W11" t="n">
-        <v>4.389838644419843</v>
+        <v>4.35725967437622</v>
       </c>
       <c r="X11" t="n">
-        <v>7.53591347411274</v>
+        <v>7.535858105489311</v>
       </c>
     </row>
     <row r="12">
@@ -1318,72 +1318,72 @@
         <v>9</v>
       </c>
       <c r="C12" t="n">
-        <v>163.75663950775</v>
+        <v>163.8660027232646</v>
       </c>
       <c r="D12" t="n">
-        <v>1.701384074323391</v>
+        <v>1.37627668812116</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:30.000000000</t>
+          <t>22 Jun 2025 10:15:25.000000000</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>-4.887753526715692</v>
+        <v>80.46771737025171</v>
       </c>
       <c r="G12" t="n">
-        <v>-7.898053483355504</v>
+        <v>77.45741741361189</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2844556760497847</v>
+        <v>1e-30</v>
       </c>
       <c r="I12" t="n">
-        <v>2747.235466369206</v>
+        <v>2781.50802986114</v>
       </c>
       <c r="J12" t="n">
-        <v>-6.154164088468002</v>
+        <v>79.3089954786324</v>
       </c>
       <c r="K12" t="n">
-        <v>187.3327283013185</v>
+        <v>187.4404169714515</v>
       </c>
       <c r="L12" t="n">
-        <v>65.65411757239968</v>
+        <v>0.06804051505671602</v>
       </c>
       <c r="M12" t="n">
-        <v>-91.40932191637033</v>
+        <v>-18.12506882628442</v>
       </c>
       <c r="N12" t="n">
-        <v>-36.154164088468</v>
+        <v>49.3089954786324</v>
       </c>
       <c r="O12" t="n">
         <v>30</v>
       </c>
       <c r="P12" t="n">
-        <v>-193.4868923897865</v>
+        <v>-108.1314214928191</v>
       </c>
       <c r="Q12" t="n">
-        <v>-193.4868923897865</v>
+        <v>-108.1314214928191</v>
       </c>
       <c r="R12" t="n">
-        <v>4125.992032816553</v>
+        <v>4095.481788411548</v>
       </c>
       <c r="S12" t="n">
-        <v>777.5789358022793</v>
+        <v>780.6120045226403</v>
       </c>
       <c r="T12" t="n">
-        <v>-5609.371679543818</v>
+        <v>-5631.27161490884</v>
       </c>
       <c r="U12" t="n">
-        <v>6.090290861082371</v>
+        <v>6.114036585211042</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.608865205326335</v>
+        <v>-0.6043646888073327</v>
       </c>
       <c r="W12" t="n">
-        <v>4.396339351752002</v>
+        <v>4.363785500925694</v>
       </c>
       <c r="X12" t="n">
-        <v>7.535924582067136</v>
+        <v>7.535869156272923</v>
       </c>
     </row>
     <row r="13">
@@ -1394,72 +1394,72 @@
         <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>163.7344892568628</v>
+        <v>163.8660027232646</v>
       </c>
       <c r="D13" t="n">
-        <v>1.766912749526274</v>
+        <v>1.37627668812116</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:31.000000000</t>
+          <t>22 Jun 2025 10:15:25.000000000</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>-0.6146595022972371</v>
+        <v>97.35482661695511</v>
       </c>
       <c r="G13" t="n">
-        <v>-3.624959458937049</v>
+        <v>94.3445266603153</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1757508252713766</v>
+        <v>1e-30</v>
       </c>
       <c r="I13" t="n">
-        <v>2740.382141405968</v>
+        <v>2781.50802986114</v>
       </c>
       <c r="J13" t="n">
-        <v>-1.902765181853653</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K13" t="n">
-        <v>187.3110331835144</v>
+        <v>187.4404169714515</v>
       </c>
       <c r="L13" t="n">
-        <v>65.75613350906063</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>-91.52237757887316</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>-31.90276518185365</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O13" t="n">
         <v>30</v>
       </c>
       <c r="P13" t="n">
-        <v>-189.213798365368</v>
+        <v>-91.2443122461157</v>
       </c>
       <c r="Q13" t="n">
-        <v>-189.213798365368</v>
+        <v>-91.2443122461157</v>
       </c>
       <c r="R13" t="n">
-        <v>4132.079809975929</v>
+        <v>4095.481788411548</v>
       </c>
       <c r="S13" t="n">
-        <v>776.969623030387</v>
+        <v>780.6120045226403</v>
       </c>
       <c r="T13" t="n">
-        <v>-5604.9721781978</v>
+        <v>-5631.27161490884</v>
       </c>
       <c r="U13" t="n">
-        <v>6.085520483765377</v>
+        <v>6.114036585211042</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.6097632235579635</v>
+        <v>-0.6043646888073327</v>
       </c>
       <c r="W13" t="n">
-        <v>4.402835012545466</v>
+        <v>4.363785500925694</v>
       </c>
       <c r="X13" t="n">
-        <v>7.535935701346451</v>
+        <v>7.535869156272923</v>
       </c>
     </row>
     <row r="14">
@@ -1470,72 +1470,72 @@
         <v>9</v>
       </c>
       <c r="C14" t="n">
-        <v>163.7122446700199</v>
+        <v>163.844312670568</v>
       </c>
       <c r="D14" t="n">
-        <v>1.83261339586689</v>
+        <v>1.440964134184426</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:32.000000000</t>
+          <t>22 Jun 2025 10:15:26.000000000</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>-12.8200314266015</v>
+        <v>80.33004762409207</v>
       </c>
       <c r="G14" t="n">
-        <v>-15.83033138324131</v>
+        <v>77.31974766745226</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4096058264008593</v>
+        <v>1e-30</v>
       </c>
       <c r="I14" t="n">
-        <v>2733.529239295291</v>
+        <v>2774.652762393974</v>
       </c>
       <c r="J14" t="n">
-        <v>-14.12988520487244</v>
+        <v>79.14989218182504</v>
       </c>
       <c r="K14" t="n">
-        <v>187.2892850847998</v>
+        <v>187.4189834208038</v>
       </c>
       <c r="L14" t="n">
-        <v>65.85835496121641</v>
+        <v>0.06822492004465684</v>
       </c>
       <c r="M14" t="n">
-        <v>-91.63593769760989</v>
+        <v>-18.13301619323165</v>
       </c>
       <c r="N14" t="n">
-        <v>-44.12988520487244</v>
+        <v>49.14989218182505</v>
       </c>
       <c r="O14" t="n">
         <v>30</v>
       </c>
       <c r="P14" t="n">
-        <v>-201.4191702896723</v>
+        <v>-108.2690912389787</v>
       </c>
       <c r="Q14" t="n">
-        <v>-201.4191702896723</v>
+        <v>-108.2690912389787</v>
       </c>
       <c r="R14" t="n">
-        <v>4138.162813305039</v>
+        <v>4101.593328551306</v>
       </c>
       <c r="S14" t="n">
-        <v>776.3594126086114</v>
+        <v>780.0071904399598</v>
       </c>
       <c r="T14" t="n">
-        <v>-5600.566183867953</v>
+        <v>-5626.904654122026</v>
       </c>
       <c r="U14" t="n">
-        <v>6.080743041552916</v>
+        <v>6.109301612947864</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.6106605437377156</v>
+        <v>-0.6052661816410934</v>
       </c>
       <c r="W14" t="n">
-        <v>4.409325619226247</v>
+        <v>4.370306318775554</v>
       </c>
       <c r="X14" t="n">
-        <v>7.535946831914168</v>
+        <v>7.535880218563409</v>
       </c>
     </row>
     <row r="15">
@@ -1546,72 +1546,72 @@
         <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>163.6899049626078</v>
+        <v>163.844312670568</v>
       </c>
       <c r="D15" t="n">
-        <v>1.898487283055201</v>
+        <v>1.440964134184426</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:33.000000000</t>
+          <t>22 Jun 2025 10:15:26.000000000</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>-2.602862649906125</v>
+        <v>97.37626016760281</v>
       </c>
       <c r="G15" t="n">
-        <v>-5.613162606545937</v>
+        <v>94.365960210963</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2293267242880865</v>
+        <v>1e-30</v>
       </c>
       <c r="I15" t="n">
-        <v>2726.676771686951</v>
+        <v>2774.652762393974</v>
       </c>
       <c r="J15" t="n">
-        <v>-3.934517733300831</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K15" t="n">
-        <v>187.2674837796761</v>
+        <v>187.4189834208038</v>
       </c>
       <c r="L15" t="n">
-        <v>65.96078084855336</v>
+        <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>-91.75000760216091</v>
+        <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>-33.93451773330084</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O15" t="n">
         <v>30</v>
       </c>
       <c r="P15" t="n">
-        <v>-191.2020015129769</v>
+        <v>-91.22287869546797</v>
       </c>
       <c r="Q15" t="n">
-        <v>-191.2020015129769</v>
+        <v>-91.22287869546797</v>
       </c>
       <c r="R15" t="n">
-        <v>4144.241035757347</v>
+        <v>4101.593328551306</v>
       </c>
       <c r="S15" t="n">
-        <v>775.7483052335207</v>
+        <v>780.0071904399598</v>
       </c>
       <c r="T15" t="n">
-        <v>-5596.153701600945</v>
+        <v>-5626.904654122026</v>
       </c>
       <c r="U15" t="n">
-        <v>6.075958539821288</v>
+        <v>6.109301612947864</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.6115571648275724</v>
+        <v>-0.6052661816410934</v>
       </c>
       <c r="W15" t="n">
-        <v>4.415811164259948</v>
+        <v>4.370306318775554</v>
       </c>
       <c r="X15" t="n">
-        <v>7.535957973733796</v>
+        <v>7.535880218563409</v>
       </c>
     </row>
     <row r="16">
@@ -1622,72 +1622,72 @@
         <v>9</v>
       </c>
       <c r="C16" t="n">
-        <v>163.6674692819926</v>
+        <v>163.8225320244808</v>
       </c>
       <c r="D16" t="n">
-        <v>1.964535681859011</v>
+        <v>1.505817370914539</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:34.000000000</t>
+          <t>22 Jun 2025 10:15:27.000000000</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>-1.352453456394781</v>
+        <v>80.18886966831069</v>
       </c>
       <c r="G16" t="n">
-        <v>-4.362753413034594</v>
+        <v>77.17856971167087</v>
       </c>
       <c r="H16" t="n">
-        <v>0.196051458253885</v>
+        <v>1e-30</v>
       </c>
       <c r="I16" t="n">
-        <v>2719.824751472531</v>
+        <v>2767.797861948103</v>
       </c>
       <c r="J16" t="n">
-        <v>-2.705963274439264</v>
+        <v>78.9872288062726</v>
       </c>
       <c r="K16" t="n">
-        <v>187.2456290450263</v>
+        <v>187.3974980010327</v>
       </c>
       <c r="L16" t="n">
-        <v>66.06341034446352</v>
+        <v>0.06841070942946754</v>
       </c>
       <c r="M16" t="n">
-        <v>-91.86459253169393</v>
+        <v>-18.14100131756784</v>
       </c>
       <c r="N16" t="n">
-        <v>-32.70596327443926</v>
+        <v>48.9872288062726</v>
       </c>
       <c r="O16" t="n">
         <v>30</v>
       </c>
       <c r="P16" t="n">
-        <v>-189.9515923194656</v>
+        <v>-108.4102691947601</v>
       </c>
       <c r="Q16" t="n">
-        <v>-189.9515923194656</v>
+        <v>-108.4102691947601</v>
       </c>
       <c r="R16" t="n">
-        <v>4150.314469700492</v>
+        <v>4107.700129693329</v>
       </c>
       <c r="S16" t="n">
-        <v>775.1363046428683</v>
+        <v>779.4014782343635</v>
       </c>
       <c r="T16" t="n">
-        <v>-5591.73473646832</v>
+        <v>-5622.531175166913</v>
       </c>
       <c r="U16" t="n">
-        <v>6.071166984422134</v>
+        <v>6.104559549405135</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.6124530813658432</v>
+        <v>-0.6061669771973957</v>
       </c>
       <c r="W16" t="n">
-        <v>4.422291640088937</v>
+        <v>4.376822120357836</v>
       </c>
       <c r="X16" t="n">
-        <v>7.535969126768791</v>
+        <v>7.535891292324466</v>
       </c>
     </row>
     <row r="17">
@@ -1698,72 +1698,72 @@
         <v>9</v>
       </c>
       <c r="C17" t="n">
-        <v>163.6449369459386</v>
+        <v>163.8225320244808</v>
       </c>
       <c r="D17" t="n">
-        <v>2.030759907970624</v>
+        <v>1.505817370914539</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:35.000000000</t>
+          <t>22 Jun 2025 10:15:27.000000000</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>-31.16600120536633</v>
+        <v>97.39774558737386</v>
       </c>
       <c r="G17" t="n">
-        <v>-34.17630116200614</v>
+        <v>94.38744563073405</v>
       </c>
       <c r="H17" t="n">
-        <v>0.4889705293547085</v>
+        <v>1e-30</v>
       </c>
       <c r="I17" t="n">
-        <v>2712.973188276437</v>
+        <v>2767.797861948103</v>
       </c>
       <c r="J17" t="n">
-        <v>-32.54141942272205</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K17" t="n">
-        <v>187.223720645715</v>
+        <v>187.3974980010327</v>
       </c>
       <c r="L17" t="n">
-        <v>66.16624218758261</v>
+        <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>-91.97969785320637</v>
+        <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>-62.54141942272206</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O17" t="n">
         <v>30</v>
       </c>
       <c r="P17" t="n">
-        <v>-219.7651400684371</v>
+        <v>-91.20139327569692</v>
       </c>
       <c r="Q17" t="n">
-        <v>-219.7651400684371</v>
+        <v>-91.20139327569692</v>
       </c>
       <c r="R17" t="n">
-        <v>4156.383109219659</v>
+        <v>4107.700129693329</v>
       </c>
       <c r="S17" t="n">
-        <v>774.5234054676559</v>
+        <v>779.4014782343635</v>
       </c>
       <c r="T17" t="n">
-        <v>-5587.309293541847</v>
+        <v>-5622.531175166913</v>
       </c>
       <c r="U17" t="n">
-        <v>6.066368379863564</v>
+        <v>6.104559549405135</v>
       </c>
       <c r="V17" t="n">
-        <v>-0.613348301156279</v>
+        <v>-0.6061669771973957</v>
       </c>
       <c r="W17" t="n">
-        <v>4.428767039181215</v>
+        <v>4.376822120357836</v>
       </c>
       <c r="X17" t="n">
-        <v>7.535980290982569</v>
+        <v>7.535891292324466</v>
       </c>
     </row>
     <row r="18">
@@ -1774,72 +1774,72 @@
         <v>9</v>
       </c>
       <c r="C18" t="n">
-        <v>163.6223070849084</v>
+        <v>163.8006601567133</v>
       </c>
       <c r="D18" t="n">
-        <v>2.097161257011595</v>
+        <v>1.570837630213995</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:36.000000000</t>
+          <t>22 Jun 2025 10:15:28.000000000</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>-1.083801881361845</v>
+        <v>80.04406648525213</v>
       </c>
       <c r="G18" t="n">
-        <v>-4.094101838001657</v>
+        <v>77.03376652861232</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1887009609035135</v>
+        <v>1e-30</v>
       </c>
       <c r="I18" t="n">
-        <v>2706.122095179903</v>
+        <v>2760.943337502153</v>
       </c>
       <c r="J18" t="n">
-        <v>-2.481182388409235</v>
+        <v>78.82088810817537</v>
       </c>
       <c r="K18" t="n">
-        <v>187.2017583560234</v>
+        <v>187.375960485994</v>
       </c>
       <c r="L18" t="n">
-        <v>66.26927544370142</v>
+        <v>0.06859787099310799</v>
       </c>
       <c r="M18" t="n">
-        <v>-92.09532905694459</v>
+        <v>-18.1488769401951</v>
       </c>
       <c r="N18" t="n">
-        <v>-32.48118238840923</v>
+        <v>48.82088810817536</v>
       </c>
       <c r="O18" t="n">
         <v>30</v>
       </c>
       <c r="P18" t="n">
-        <v>-189.6829407444326</v>
+        <v>-108.5550723778186</v>
       </c>
       <c r="Q18" t="n">
-        <v>-189.6829407444326</v>
+        <v>-108.5550723778186</v>
       </c>
       <c r="R18" t="n">
-        <v>4162.446946698016</v>
+        <v>4113.802185896458</v>
       </c>
       <c r="S18" t="n">
-        <v>773.909611442592</v>
+        <v>778.7948625917469</v>
       </c>
       <c r="T18" t="n">
-        <v>-5582.877377904444</v>
+        <v>-5618.151183058709</v>
       </c>
       <c r="U18" t="n">
-        <v>6.061562732009019</v>
+        <v>6.099810399038263</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.6142428187362168</v>
+        <v>-0.6070670833234267</v>
       </c>
       <c r="W18" t="n">
-        <v>4.435237353995545</v>
+        <v>4.383332898108165</v>
       </c>
       <c r="X18" t="n">
-        <v>7.535991466338523</v>
+        <v>7.535902377519727</v>
       </c>
     </row>
     <row r="19">
@@ -1850,72 +1850,72 @@
         <v>9</v>
       </c>
       <c r="C19" t="n">
-        <v>163.5995788196273</v>
+        <v>163.8006601567133</v>
       </c>
       <c r="D19" t="n">
-        <v>2.163741037189367</v>
+        <v>1.570837630213995</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:37.000000000</t>
+          <t>22 Jun 2025 10:15:28.000000000</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>-3.123117005461492</v>
+        <v>97.41928310241255</v>
       </c>
       <c r="G19" t="n">
-        <v>-6.133416962101304</v>
+        <v>94.40898314577274</v>
       </c>
       <c r="H19" t="n">
-        <v>0.2425942630008318</v>
+        <v>1e-30</v>
       </c>
       <c r="I19" t="n">
-        <v>2699.271485352876</v>
+        <v>2760.943337502153</v>
       </c>
       <c r="J19" t="n">
-        <v>-4.542513919596755</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K19" t="n">
-        <v>187.1797419489355</v>
+        <v>187.375960485994</v>
       </c>
       <c r="L19" t="n">
-        <v>66.37250913494523</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>-92.21149144359188</v>
+        <v>0</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.54251391959676</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O19" t="n">
         <v>30</v>
       </c>
       <c r="P19" t="n">
-        <v>-191.7222558685323</v>
+        <v>-91.17985576065823</v>
       </c>
       <c r="Q19" t="n">
-        <v>-191.7222558685323</v>
+        <v>-91.17985576065823</v>
       </c>
       <c r="R19" t="n">
-        <v>4168.505974541447</v>
+        <v>4113.802185896458</v>
       </c>
       <c r="S19" t="n">
-        <v>773.2949263188161</v>
+        <v>778.7948625917469</v>
       </c>
       <c r="T19" t="n">
-        <v>-5578.438994635303</v>
+        <v>-5618.151183058709</v>
       </c>
       <c r="U19" t="n">
-        <v>6.056750046720541</v>
+        <v>6.099810399038263</v>
       </c>
       <c r="V19" t="n">
-        <v>-0.6151366286611197</v>
+        <v>-0.6070670833234267</v>
       </c>
       <c r="W19" t="n">
-        <v>4.441702577012514</v>
+        <v>4.383332898108165</v>
       </c>
       <c r="X19" t="n">
-        <v>7.536002652800055</v>
+        <v>7.535902377519727</v>
       </c>
     </row>
     <row r="20">
@@ -1926,72 +1926,72 @@
         <v>9</v>
       </c>
       <c r="C20" t="n">
-        <v>163.5767514431665</v>
+        <v>163.778696257454</v>
       </c>
       <c r="D20" t="n">
-        <v>2.230500602020815</v>
+        <v>1.636026123521759</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:38.000000000</t>
+          <t>22 Jun 2025 10:15:29.000000000</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>-9.939475079640626</v>
+        <v>79.89546803055553</v>
       </c>
       <c r="G20" t="n">
-        <v>-12.94977503628044</v>
+        <v>76.88516807391572</v>
       </c>
       <c r="H20" t="n">
-        <v>0.3750759811161913</v>
+        <v>1e-30</v>
       </c>
       <c r="I20" t="n">
-        <v>2692.421368734845</v>
+        <v>2754.089201487097</v>
       </c>
       <c r="J20" t="n">
-        <v>-11.38094275729157</v>
+        <v>78.6506998263211</v>
       </c>
       <c r="K20" t="n">
-        <v>187.1576711854198</v>
+        <v>187.3543706588364</v>
       </c>
       <c r="L20" t="n">
-        <v>66.47594190378032</v>
+        <v>0.06878644318451023</v>
       </c>
       <c r="M20" t="n">
-        <v>-92.32819046213007</v>
+        <v>-18.15678873931403</v>
       </c>
       <c r="N20" t="n">
-        <v>-41.38094275729158</v>
+        <v>48.6506998263211</v>
       </c>
       <c r="O20" t="n">
         <v>30</v>
       </c>
       <c r="P20" t="n">
-        <v>-198.5386139427114</v>
+        <v>-108.7036708325152</v>
       </c>
       <c r="Q20" t="n">
-        <v>-198.5386139427114</v>
+        <v>-108.7036708325152</v>
       </c>
       <c r="R20" t="n">
-        <v>4174.560186828104</v>
+        <v>4119.899489477398</v>
       </c>
       <c r="S20" t="n">
-        <v>772.6793447066512</v>
+        <v>778.1873472104074</v>
       </c>
       <c r="T20" t="n">
-        <v>-5573.994148843788</v>
+        <v>-5613.764682845886</v>
       </c>
       <c r="U20" t="n">
-        <v>6.051930328543438</v>
+        <v>6.095054167668101</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.6160297387119786</v>
+        <v>-0.6079664945240202</v>
       </c>
       <c r="W20" t="n">
-        <v>4.448162700694659</v>
+        <v>4.389838644419843</v>
       </c>
       <c r="X20" t="n">
-        <v>7.536013850330467</v>
+        <v>7.53591347411274</v>
       </c>
     </row>
     <row r="21">
@@ -2002,72 +2002,72 @@
         <v>9</v>
       </c>
       <c r="C21" t="n">
-        <v>163.5538240585597</v>
+        <v>163.778696257454</v>
       </c>
       <c r="D21" t="n">
-        <v>2.29744128560822</v>
+        <v>1.636026123521759</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:39.000000000</t>
+          <t>22 Jun 2025 10:15:29.000000000</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>-0.3727488427323288</v>
+        <v>97.4408729295702</v>
       </c>
       <c r="G21" t="n">
-        <v>-3.383048799372141</v>
+        <v>94.43057297293039</v>
       </c>
       <c r="H21" t="n">
-        <v>0.1690330243386668</v>
+        <v>1e-30</v>
       </c>
       <c r="I21" t="n">
-        <v>2685.571758676042</v>
+        <v>2754.089201487097</v>
       </c>
       <c r="J21" t="n">
-        <v>-1.836341870042522</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K21" t="n">
-        <v>187.1355458357606</v>
+        <v>187.3543706588364</v>
       </c>
       <c r="L21" t="n">
-        <v>66.57957272238016</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>-92.44543168252352</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>-31.83634187004252</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O21" t="n">
         <v>30</v>
       </c>
       <c r="P21" t="n">
-        <v>-188.9718877058031</v>
+        <v>-91.15826593350057</v>
       </c>
       <c r="Q21" t="n">
-        <v>-188.9718877058031</v>
+        <v>-91.15826593350057</v>
       </c>
       <c r="R21" t="n">
-        <v>4180.609575994578</v>
+        <v>4119.899489477398</v>
       </c>
       <c r="S21" t="n">
-        <v>772.0628703534514</v>
+        <v>778.1873472104074</v>
       </c>
       <c r="T21" t="n">
-        <v>-5569.542845609092</v>
+        <v>-5613.764682845886</v>
       </c>
       <c r="U21" t="n">
-        <v>6.047103583339349</v>
+        <v>6.095054167668101</v>
       </c>
       <c r="V21" t="n">
-        <v>-0.6169221434443384</v>
+        <v>-0.6079664945240202</v>
       </c>
       <c r="W21" t="n">
-        <v>4.454617717555306</v>
+        <v>4.389838644419843</v>
       </c>
       <c r="X21" t="n">
-        <v>7.536025058893129</v>
+        <v>7.53591347411274</v>
       </c>
     </row>
     <row r="22">
@@ -2078,72 +2078,72 @@
         <v>9</v>
       </c>
       <c r="C22" t="n">
-        <v>163.5307958202829</v>
+        <v>163.75663950775</v>
       </c>
       <c r="D22" t="n">
-        <v>2.364564445292875</v>
+        <v>1.701384074323391</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:40.000000000</t>
+          <t>22 Jun 2025 10:15:30.000000000</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>-7.041474527999783</v>
+        <v>79.74291598209798</v>
       </c>
       <c r="G22" t="n">
-        <v>-10.0517744846396</v>
+        <v>76.73261602545817</v>
       </c>
       <c r="H22" t="n">
-        <v>0.3283204004403988</v>
+        <v>1e-30</v>
       </c>
       <c r="I22" t="n">
-        <v>2678.72266758524</v>
+        <v>2747.235466369206</v>
       </c>
       <c r="J22" t="n">
-        <v>-8.527247725500356</v>
+        <v>78.47650542034567</v>
       </c>
       <c r="K22" t="n">
-        <v>187.1133656655702</v>
+        <v>187.3327283013185</v>
       </c>
       <c r="L22" t="n">
-        <v>66.68340045339963</v>
+        <v>0.06897644046812162</v>
       </c>
       <c r="M22" t="n">
-        <v>-92.56322047294749</v>
+        <v>-18.16473643420527</v>
       </c>
       <c r="N22" t="n">
-        <v>-38.52724772550035</v>
+        <v>48.47650542034567</v>
       </c>
       <c r="O22" t="n">
         <v>30</v>
       </c>
       <c r="P22" t="n">
-        <v>-195.6406133910706</v>
+        <v>-108.8562228809728</v>
       </c>
       <c r="Q22" t="n">
-        <v>-195.6406133910706</v>
+        <v>-108.8562228809728</v>
       </c>
       <c r="R22" t="n">
-        <v>4186.654134981074</v>
+        <v>4125.992032816553</v>
       </c>
       <c r="S22" t="n">
-        <v>771.4455039683504</v>
+        <v>777.5789358022793</v>
       </c>
       <c r="T22" t="n">
-        <v>-5565.085090068063</v>
+        <v>-5609.371679543818</v>
       </c>
       <c r="U22" t="n">
-        <v>6.042269816583015</v>
+        <v>6.090290861082371</v>
       </c>
       <c r="V22" t="n">
-        <v>-0.6178138418177311</v>
+        <v>-0.608865205326335</v>
       </c>
       <c r="W22" t="n">
-        <v>4.461067620043642</v>
+        <v>4.396339351752002</v>
       </c>
       <c r="X22" t="n">
-        <v>7.536036278451264</v>
+        <v>7.535924582067136</v>
       </c>
     </row>
     <row r="23">
@@ -2154,72 +2154,72 @@
         <v>9</v>
       </c>
       <c r="C23" t="n">
-        <v>163.5076658118871</v>
+        <v>163.75663950775</v>
       </c>
       <c r="D23" t="n">
-        <v>2.431871441127972</v>
+        <v>1.701384074323391</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:41.000000000</t>
+          <t>22 Jun 2025 10:15:30.000000000</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>-4.272057343231566</v>
+        <v>97.4625152870881</v>
       </c>
       <c r="G23" t="n">
-        <v>-7.282357299871377</v>
+        <v>94.45221533044828</v>
       </c>
       <c r="H23" t="n">
-        <v>0.2704339964213588</v>
+        <v>1e-30</v>
       </c>
       <c r="I23" t="n">
-        <v>2671.87410903505</v>
+        <v>2747.235466369206</v>
       </c>
       <c r="J23" t="n">
-        <v>-5.780065763723331</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K23" t="n">
-        <v>187.091130442579</v>
+        <v>187.3327283013185</v>
       </c>
       <c r="L23" t="n">
-        <v>66.78742388347355</v>
+        <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>-92.6815624057221</v>
+        <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>-35.78006576372333</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O23" t="n">
         <v>30</v>
       </c>
       <c r="P23" t="n">
-        <v>-192.8711962063024</v>
+        <v>-91.13662357598271</v>
       </c>
       <c r="Q23" t="n">
-        <v>-192.8711962063024</v>
+        <v>-91.13662357598271</v>
       </c>
       <c r="R23" t="n">
-        <v>4192.693856232201</v>
+        <v>4125.992032816553</v>
       </c>
       <c r="S23" t="n">
-        <v>770.8272493231128</v>
+        <v>777.5789358022793</v>
       </c>
       <c r="T23" t="n">
-        <v>-5560.620887318662</v>
+        <v>-5609.371679543818</v>
       </c>
       <c r="U23" t="n">
-        <v>6.037429034159843</v>
+        <v>6.090290861082371</v>
       </c>
       <c r="V23" t="n">
-        <v>-0.6187048284063847</v>
+        <v>-0.608865205326335</v>
       </c>
       <c r="W23" t="n">
-        <v>4.467512400678472</v>
+        <v>4.396339351752002</v>
       </c>
       <c r="X23" t="n">
-        <v>7.536047508968182</v>
+        <v>7.535924582067136</v>
       </c>
     </row>
     <row r="24">
@@ -2230,72 +2230,72 @@
         <v>9</v>
       </c>
       <c r="C24" t="n">
-        <v>163.4844332917572</v>
+        <v>163.7344892568628</v>
       </c>
       <c r="D24" t="n">
-        <v>2.499363679460058</v>
+        <v>1.766912749526274</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:42.000000000</t>
+          <t>22 Jun 2025 10:15:31.000000000</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>-0.6834817026172546</v>
+        <v>79.58626747791173</v>
       </c>
       <c r="G24" t="n">
-        <v>-3.693781659257067</v>
+        <v>76.57596752127192</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1776578940232714</v>
+        <v>1e-30</v>
       </c>
       <c r="I24" t="n">
-        <v>2665.026093371957</v>
+        <v>2740.382141405968</v>
       </c>
       <c r="J24" t="n">
-        <v>-2.213780643327852</v>
+        <v>78.29816179835531</v>
       </c>
       <c r="K24" t="n">
-        <v>187.0688399223602</v>
+        <v>187.3110331835144</v>
       </c>
       <c r="L24" t="n">
-        <v>66.89164151904944</v>
+        <v>0.06916785032035556</v>
       </c>
       <c r="M24" t="n">
-        <v>-92.80046302597869</v>
+        <v>-18.17257223690649</v>
       </c>
       <c r="N24" t="n">
-        <v>-32.21378064332785</v>
+        <v>48.29816179835532</v>
       </c>
       <c r="O24" t="n">
         <v>30</v>
       </c>
       <c r="P24" t="n">
-        <v>-189.282620565688</v>
+        <v>-109.0128713851591</v>
       </c>
       <c r="Q24" t="n">
-        <v>-189.282620565688</v>
+        <v>-109.0128713851591</v>
       </c>
       <c r="R24" t="n">
-        <v>4198.728733844372</v>
+        <v>4132.079809975929</v>
       </c>
       <c r="S24" t="n">
-        <v>770.2081009969961</v>
+        <v>776.969623030387</v>
       </c>
       <c r="T24" t="n">
-        <v>-5556.150242500321</v>
+        <v>-5604.9721781978</v>
       </c>
       <c r="U24" t="n">
-        <v>6.032581240642913</v>
+        <v>6.085520483765377</v>
       </c>
       <c r="V24" t="n">
-        <v>-0.6195951109660709</v>
+        <v>-0.6097632235579635</v>
       </c>
       <c r="W24" t="n">
-        <v>4.473952051944367</v>
+        <v>4.402835012545466</v>
       </c>
       <c r="X24" t="n">
-        <v>7.536058750407076</v>
+        <v>7.535935701346451</v>
       </c>
     </row>
     <row r="25">
@@ -2306,72 +2306,72 @@
         <v>9</v>
       </c>
       <c r="C25" t="n">
-        <v>163.46109732498</v>
+        <v>163.7344892568628</v>
       </c>
       <c r="D25" t="n">
-        <v>2.567042547016628</v>
+        <v>1.766912749526274</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:43.000000000</t>
+          <t>22 Jun 2025 10:15:31.000000000</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>-20.0416774482284</v>
+        <v>97.4842104048922</v>
       </c>
       <c r="G25" t="n">
-        <v>-23.05197740486822</v>
+        <v>94.47391044825238</v>
       </c>
       <c r="H25" t="n">
-        <v>0.4603621805145561</v>
+        <v>1e-30</v>
       </c>
       <c r="I25" t="n">
-        <v>2658.178634404458</v>
+        <v>2740.382141405968</v>
       </c>
       <c r="J25" t="n">
-        <v>-21.59432244126616</v>
+        <v>96.19610472533579</v>
       </c>
       <c r="K25" t="n">
-        <v>187.046493870033</v>
+        <v>187.3110331835144</v>
       </c>
       <c r="L25" t="n">
-        <v>66.99605236256065</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>-92.91992784732427</v>
+        <v>0</v>
       </c>
       <c r="N25" t="n">
-        <v>-51.59432244126616</v>
+        <v>66.19610472533577</v>
       </c>
       <c r="O25" t="n">
         <v>30</v>
       </c>
       <c r="P25" t="n">
-        <v>-208.6408163112992</v>
+        <v>-91.11492845817861</v>
       </c>
       <c r="Q25" t="n">
-        <v>-208.6408163112992</v>
+        <v>-91.11492845817861</v>
       </c>
       <c r="R25" t="n">
-        <v>4204.758760252277</v>
+        <v>4132.079809975929</v>
       </c>
       <c r="S25" t="n">
-        <v>769.5880627614288</v>
+        <v>776.969623030387</v>
       </c>
       <c r="T25" t="n">
-        <v>-5551.67316074104</v>
+        <v>-5604.9721781978</v>
       </c>
       <c r="U25" t="n">
-        <v>6.027726441949745</v>
+        <v>6.085520483765377</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.6204846840661218</v>
+        <v>-0.6097632235579635</v>
       </c>
       <c r="W25" t="n">
-        <v>4.480386566349355</v>
+        <v>4.402835012545466</v>
       </c>
       <c r="X25" t="n">
-        <v>7.536070002731167</v>
+        <v>7.535935701346451</v>
       </c>
     </row>
     <row r="26">
@@ -2382,72 +2382,72 @@
         <v>9</v>
       </c>
       <c r="C26" t="n">
-        <v>163.4376569660906</v>
+        <v>163.7122446700199</v>
       </c>
       <c r="D26" t="n">
-        <v>2.634909443945261</v>
+        <v>1.83261339586689</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>22 Jun 2025 10:15:44.000000000</t>
+          <t>22 Jun 2025 10:15:32.000000000</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>-1.383049052874487</v>
+        <v>79.42532064437358</v>
       </c>
       <c r="G26" t="n">
-        <v>-4.393349009514299</v>
+        <v>76.41502068773377</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1968849188393932</v>
+        <v>1e-30</v>
       </c>
       <c r="I26" t="n">
-        <v>2651.331746062029</v>
+        <v>2733.529239295291</v>
       </c>
       <c r="J26" t="n">
-        <v>-2.958095866498614</v>
+        <v>78.11546686610265</v>
       </c>
       <c r="K26" t="n">
-        <v>187.0240920494467</v>
+        <v>187.2892850847998</v>
       </c>
       <c r="L26" t="n">
-        <v>67.10065503623181</v>
+        <v>0.06936071250274915</v>
       </c>
       <c r="M26" t="n">
-        <v>-93.03996248404185</v>
+        <v>-18.18044230957038</v>
       </c>
       <c r="N26" t="n">
-        <v>-32.95809586649861</v>
+        <v>48.11546686610265</v>
       </c>
       <c r="O26" t="n">
         <v>30</v>
       </c>
       <c r="P26" t="n">
-        <v>-189.9821879159453</v>
+        <v>-109.1738182186972</v>
       </c>
       <c r="Q26" t="n">
-        <v>-189.9821879159453</v>
+        <v>-109.1738182186972</v>
       </c>
       <c r="R26" t="n">
-        <v>4210.783927892788</v>
+        <v>4138.162813305039</v>
       </c>
       <c r="S26" t="n">
-        <v>768.9671384068922</v>
+        <v>776.3594126086114</v>
       </c>
       <c r="T26" t="n">
-        <v>-5547.189647180097</v>
+        <v>-5600.566183867953</v>
       </c>
       <c r="U26" t="n">
-        <v>6.022864644012732</v>
+        <v>6.080743041552916</v>
       </c>
       <c r="V26" t="n">
-        <v>-0.621373542290163</v>
+        <v>-0.6106605437377156</v>
       </c>
       <c r="W26" t="n">
-        <v>4.486815936401529</v>
+        <v>4.409325619226247</v>
       </c>
       <c r="X26" t="n">
-        <v>7.536081265903624</v>
+        <v>7.535946831914168</v>
       </c>
     </row>
     <row r="27">
@@ -2458,71 +2458,1971 @@
         <v>9</v>
       </c>
       <c r="C27" t="n">
+        <v>163.7122446700199</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.83261339586689</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:32.000000000</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>97.50595850360671</v>
+      </c>
+      <c r="G27" t="n">
+        <v>94.49565854696689</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I27" t="n">
+        <v>2733.529239295291</v>
+      </c>
+      <c r="J27" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K27" t="n">
+        <v>187.2892850847998</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O27" t="n">
+        <v>30</v>
+      </c>
+      <c r="P27" t="n">
+        <v>-91.09318035946407</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>-91.09318035946407</v>
+      </c>
+      <c r="R27" t="n">
+        <v>4138.162813305039</v>
+      </c>
+      <c r="S27" t="n">
+        <v>776.3594126086114</v>
+      </c>
+      <c r="T27" t="n">
+        <v>-5600.566183867953</v>
+      </c>
+      <c r="U27" t="n">
+        <v>6.080743041552916</v>
+      </c>
+      <c r="V27" t="n">
+        <v>-0.6106605437377156</v>
+      </c>
+      <c r="W27" t="n">
+        <v>4.409325619226247</v>
+      </c>
+      <c r="X27" t="n">
+        <v>7.535946831914168</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>9</v>
+      </c>
+      <c r="C28" t="n">
+        <v>163.6899049626078</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.898487283055201</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:33.000000000</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>79.25989332290443</v>
+      </c>
+      <c r="G28" t="n">
+        <v>76.24959336626462</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I28" t="n">
+        <v>2726.676771686951</v>
+      </c>
+      <c r="J28" t="n">
+        <v>77.92823823950971</v>
+      </c>
+      <c r="K28" t="n">
+        <v>187.2674837796761</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.06955503281299077</v>
+      </c>
+      <c r="M28" t="n">
+        <v>-18.18829705525783</v>
+      </c>
+      <c r="N28" t="n">
+        <v>47.92823823950972</v>
+      </c>
+      <c r="O28" t="n">
+        <v>30</v>
+      </c>
+      <c r="P28" t="n">
+        <v>-109.3392455401664</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>-109.3392455401664</v>
+      </c>
+      <c r="R28" t="n">
+        <v>4144.241035757347</v>
+      </c>
+      <c r="S28" t="n">
+        <v>775.7483052335207</v>
+      </c>
+      <c r="T28" t="n">
+        <v>-5596.153701600945</v>
+      </c>
+      <c r="U28" t="n">
+        <v>6.075958539821288</v>
+      </c>
+      <c r="V28" t="n">
+        <v>-0.6115571648275724</v>
+      </c>
+      <c r="W28" t="n">
+        <v>4.415811164259948</v>
+      </c>
+      <c r="X28" t="n">
+        <v>7.535957973733796</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>9</v>
+      </c>
+      <c r="C29" t="n">
+        <v>163.6899049626078</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.898487283055201</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:33.000000000</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>97.52775980873048</v>
+      </c>
+      <c r="G29" t="n">
+        <v>94.51745985209067</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I29" t="n">
+        <v>2726.676771686951</v>
+      </c>
+      <c r="J29" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K29" t="n">
+        <v>187.2674837796761</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O29" t="n">
+        <v>30</v>
+      </c>
+      <c r="P29" t="n">
+        <v>-91.0713790543403</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>-91.0713790543403</v>
+      </c>
+      <c r="R29" t="n">
+        <v>4144.241035757347</v>
+      </c>
+      <c r="S29" t="n">
+        <v>775.7483052335207</v>
+      </c>
+      <c r="T29" t="n">
+        <v>-5596.153701600945</v>
+      </c>
+      <c r="U29" t="n">
+        <v>6.075958539821288</v>
+      </c>
+      <c r="V29" t="n">
+        <v>-0.6115571648275724</v>
+      </c>
+      <c r="W29" t="n">
+        <v>4.415811164259948</v>
+      </c>
+      <c r="X29" t="n">
+        <v>7.535957973733796</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>9</v>
+      </c>
+      <c r="C30" t="n">
+        <v>163.6674692819926</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.964535681859011</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:34.000000000</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>79.08977421483648</v>
+      </c>
+      <c r="G30" t="n">
+        <v>76.07947425819665</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I30" t="n">
+        <v>2719.824751472531</v>
+      </c>
+      <c r="J30" t="n">
+        <v>77.736264396792</v>
+      </c>
+      <c r="K30" t="n">
+        <v>187.2456290450263</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.06975083417806519</v>
+      </c>
+      <c r="M30" t="n">
+        <v>-18.19618503579261</v>
+      </c>
+      <c r="N30" t="n">
+        <v>47.736264396792</v>
+      </c>
+      <c r="O30" t="n">
+        <v>30</v>
+      </c>
+      <c r="P30" t="n">
+        <v>-109.5093646482343</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>-109.5093646482343</v>
+      </c>
+      <c r="R30" t="n">
+        <v>4150.314469700492</v>
+      </c>
+      <c r="S30" t="n">
+        <v>775.1363046428683</v>
+      </c>
+      <c r="T30" t="n">
+        <v>-5591.73473646832</v>
+      </c>
+      <c r="U30" t="n">
+        <v>6.071166984422134</v>
+      </c>
+      <c r="V30" t="n">
+        <v>-0.6124530813658432</v>
+      </c>
+      <c r="W30" t="n">
+        <v>4.422291640088937</v>
+      </c>
+      <c r="X30" t="n">
+        <v>7.535969126768791</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>9</v>
+      </c>
+      <c r="C31" t="n">
+        <v>163.6674692819926</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.964535681859011</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:34.000000000</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>97.54961454338027</v>
+      </c>
+      <c r="G31" t="n">
+        <v>94.53931458674046</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I31" t="n">
+        <v>2719.824751472531</v>
+      </c>
+      <c r="J31" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K31" t="n">
+        <v>187.2456290450263</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O31" t="n">
+        <v>30</v>
+      </c>
+      <c r="P31" t="n">
+        <v>-91.04952431969053</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>-91.04952431969053</v>
+      </c>
+      <c r="R31" t="n">
+        <v>4150.314469700492</v>
+      </c>
+      <c r="S31" t="n">
+        <v>775.1363046428683</v>
+      </c>
+      <c r="T31" t="n">
+        <v>-5591.73473646832</v>
+      </c>
+      <c r="U31" t="n">
+        <v>6.071166984422134</v>
+      </c>
+      <c r="V31" t="n">
+        <v>-0.6124530813658432</v>
+      </c>
+      <c r="W31" t="n">
+        <v>4.422291640088937</v>
+      </c>
+      <c r="X31" t="n">
+        <v>7.535969126768791</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>9</v>
+      </c>
+      <c r="C32" t="n">
+        <v>163.6449369459386</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2.030759907970624</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:35.000000000</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>78.91477279939242</v>
+      </c>
+      <c r="G32" t="n">
+        <v>75.90447284275261</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I32" t="n">
+        <v>2712.973188276437</v>
+      </c>
+      <c r="J32" t="n">
+        <v>77.53935458203669</v>
+      </c>
+      <c r="K32" t="n">
+        <v>187.223720645715</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.06994810444971686</v>
+      </c>
+      <c r="M32" t="n">
+        <v>-18.20395782957884</v>
+      </c>
+      <c r="N32" t="n">
+        <v>47.5393545820367</v>
+      </c>
+      <c r="O32" t="n">
+        <v>30</v>
+      </c>
+      <c r="P32" t="n">
+        <v>-109.6843660636784</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>-109.6843660636784</v>
+      </c>
+      <c r="R32" t="n">
+        <v>4156.383109219659</v>
+      </c>
+      <c r="S32" t="n">
+        <v>774.5234054676559</v>
+      </c>
+      <c r="T32" t="n">
+        <v>-5587.309293541847</v>
+      </c>
+      <c r="U32" t="n">
+        <v>6.066368379863564</v>
+      </c>
+      <c r="V32" t="n">
+        <v>-0.613348301156279</v>
+      </c>
+      <c r="W32" t="n">
+        <v>4.428767039181215</v>
+      </c>
+      <c r="X32" t="n">
+        <v>7.535980290982569</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>9</v>
+      </c>
+      <c r="C33" t="n">
+        <v>163.6449369459386</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2.030759907970624</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:35.000000000</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>97.5715229426915</v>
+      </c>
+      <c r="G33" t="n">
+        <v>94.56122298605169</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I33" t="n">
+        <v>2712.973188276437</v>
+      </c>
+      <c r="J33" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K33" t="n">
+        <v>187.223720645715</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O33" t="n">
+        <v>30</v>
+      </c>
+      <c r="P33" t="n">
+        <v>-91.02761592037929</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>-91.02761592037929</v>
+      </c>
+      <c r="R33" t="n">
+        <v>4156.383109219659</v>
+      </c>
+      <c r="S33" t="n">
+        <v>774.5234054676559</v>
+      </c>
+      <c r="T33" t="n">
+        <v>-5587.309293541847</v>
+      </c>
+      <c r="U33" t="n">
+        <v>6.066368379863564</v>
+      </c>
+      <c r="V33" t="n">
+        <v>-0.613348301156279</v>
+      </c>
+      <c r="W33" t="n">
+        <v>4.428767039181215</v>
+      </c>
+      <c r="X33" t="n">
+        <v>7.535980290982569</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>9</v>
+      </c>
+      <c r="C34" t="n">
+        <v>163.6223070849084</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2.097161257011595</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:36.000000000</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>78.73463046121852</v>
+      </c>
+      <c r="G34" t="n">
+        <v>75.7243305045787</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I34" t="n">
+        <v>2706.122095179903</v>
+      </c>
+      <c r="J34" t="n">
+        <v>77.33724995417111</v>
+      </c>
+      <c r="K34" t="n">
+        <v>187.2017583560234</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.07014688485007028</v>
+      </c>
+      <c r="M34" t="n">
+        <v>-18.21176218102651</v>
+      </c>
+      <c r="N34" t="n">
+        <v>47.33724995417112</v>
+      </c>
+      <c r="O34" t="n">
+        <v>30</v>
+      </c>
+      <c r="P34" t="n">
+        <v>-109.8645084018523</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>-109.8645084018523</v>
+      </c>
+      <c r="R34" t="n">
+        <v>4162.446946698016</v>
+      </c>
+      <c r="S34" t="n">
+        <v>773.909611442592</v>
+      </c>
+      <c r="T34" t="n">
+        <v>-5582.877377904444</v>
+      </c>
+      <c r="U34" t="n">
+        <v>6.061562732009019</v>
+      </c>
+      <c r="V34" t="n">
+        <v>-0.6142428187362168</v>
+      </c>
+      <c r="W34" t="n">
+        <v>4.435237353995545</v>
+      </c>
+      <c r="X34" t="n">
+        <v>7.535991466338523</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>9</v>
+      </c>
+      <c r="C35" t="n">
+        <v>163.6223070849084</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2.097161257011595</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:36.000000000</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>97.59348523238316</v>
+      </c>
+      <c r="G35" t="n">
+        <v>94.58318527574335</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2706.122095179903</v>
+      </c>
+      <c r="J35" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K35" t="n">
+        <v>187.2017583560234</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O35" t="n">
+        <v>30</v>
+      </c>
+      <c r="P35" t="n">
+        <v>-91.00565363068762</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>-91.00565363068762</v>
+      </c>
+      <c r="R35" t="n">
+        <v>4162.446946698016</v>
+      </c>
+      <c r="S35" t="n">
+        <v>773.909611442592</v>
+      </c>
+      <c r="T35" t="n">
+        <v>-5582.877377904444</v>
+      </c>
+      <c r="U35" t="n">
+        <v>6.061562732009019</v>
+      </c>
+      <c r="V35" t="n">
+        <v>-0.6142428187362168</v>
+      </c>
+      <c r="W35" t="n">
+        <v>4.435237353995545</v>
+      </c>
+      <c r="X35" t="n">
+        <v>7.535991466338523</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>9</v>
+      </c>
+      <c r="C36" t="n">
+        <v>163.5995788196273</v>
+      </c>
+      <c r="D36" t="n">
+        <v>2.163741037189367</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:37.000000000</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>78.54909696743688</v>
+      </c>
+      <c r="G36" t="n">
+        <v>75.53879701079707</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I36" t="n">
+        <v>2699.271485352876</v>
+      </c>
+      <c r="J36" t="n">
+        <v>77.12970005330162</v>
+      </c>
+      <c r="K36" t="n">
+        <v>187.1797419489355</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.07034719059619075</v>
+      </c>
+      <c r="M36" t="n">
+        <v>-18.21959767816955</v>
+      </c>
+      <c r="N36" t="n">
+        <v>47.12970005330162</v>
+      </c>
+      <c r="O36" t="n">
+        <v>30</v>
+      </c>
+      <c r="P36" t="n">
+        <v>-110.0500418956339</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>-110.0500418956339</v>
+      </c>
+      <c r="R36" t="n">
+        <v>4168.505974541447</v>
+      </c>
+      <c r="S36" t="n">
+        <v>773.2949263188161</v>
+      </c>
+      <c r="T36" t="n">
+        <v>-5578.438994635303</v>
+      </c>
+      <c r="U36" t="n">
+        <v>6.056750046720541</v>
+      </c>
+      <c r="V36" t="n">
+        <v>-0.6151366286611197</v>
+      </c>
+      <c r="W36" t="n">
+        <v>4.441702577012514</v>
+      </c>
+      <c r="X36" t="n">
+        <v>7.536002652800055</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>9</v>
+      </c>
+      <c r="C37" t="n">
+        <v>163.5995788196273</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2.163741037189367</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:37.000000000</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>97.61550163947105</v>
+      </c>
+      <c r="G37" t="n">
+        <v>94.60520168283124</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I37" t="n">
+        <v>2699.271485352876</v>
+      </c>
+      <c r="J37" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K37" t="n">
+        <v>187.1797419489355</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O37" t="n">
+        <v>30</v>
+      </c>
+      <c r="P37" t="n">
+        <v>-90.98363722359976</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>-90.98363722359976</v>
+      </c>
+      <c r="R37" t="n">
+        <v>4168.505974541447</v>
+      </c>
+      <c r="S37" t="n">
+        <v>773.2949263188161</v>
+      </c>
+      <c r="T37" t="n">
+        <v>-5578.438994635303</v>
+      </c>
+      <c r="U37" t="n">
+        <v>6.056750046720541</v>
+      </c>
+      <c r="V37" t="n">
+        <v>-0.6151366286611197</v>
+      </c>
+      <c r="W37" t="n">
+        <v>4.441702577012514</v>
+      </c>
+      <c r="X37" t="n">
+        <v>7.536002652800055</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>9</v>
+      </c>
+      <c r="C38" t="n">
+        <v>163.5767514431665</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2.230500602020815</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:38.000000000</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>78.35793327149949</v>
+      </c>
+      <c r="G38" t="n">
+        <v>75.34763331485968</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I38" t="n">
+        <v>2692.421368734845</v>
+      </c>
+      <c r="J38" t="n">
+        <v>76.91646559384853</v>
+      </c>
+      <c r="K38" t="n">
+        <v>187.1576711854198</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.07054900900560299</v>
+      </c>
+      <c r="M38" t="n">
+        <v>-18.22731541295419</v>
+      </c>
+      <c r="N38" t="n">
+        <v>46.91646559384854</v>
+      </c>
+      <c r="O38" t="n">
+        <v>30</v>
+      </c>
+      <c r="P38" t="n">
+        <v>-110.2412055915713</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>-110.2412055915713</v>
+      </c>
+      <c r="R38" t="n">
+        <v>4174.560186828104</v>
+      </c>
+      <c r="S38" t="n">
+        <v>772.6793447066512</v>
+      </c>
+      <c r="T38" t="n">
+        <v>-5573.994148843788</v>
+      </c>
+      <c r="U38" t="n">
+        <v>6.051930328543438</v>
+      </c>
+      <c r="V38" t="n">
+        <v>-0.6160297387119786</v>
+      </c>
+      <c r="W38" t="n">
+        <v>4.448162700694659</v>
+      </c>
+      <c r="X38" t="n">
+        <v>7.536013850330467</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>9</v>
+      </c>
+      <c r="C39" t="n">
+        <v>163.5767514431665</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2.230500602020815</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:38.000000000</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>97.63757240298672</v>
+      </c>
+      <c r="G39" t="n">
+        <v>94.62727244634691</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I39" t="n">
+        <v>2692.421368734845</v>
+      </c>
+      <c r="J39" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K39" t="n">
+        <v>187.1576711854198</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O39" t="n">
+        <v>30</v>
+      </c>
+      <c r="P39" t="n">
+        <v>-90.96156646008407</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>-90.96156646008407</v>
+      </c>
+      <c r="R39" t="n">
+        <v>4174.560186828104</v>
+      </c>
+      <c r="S39" t="n">
+        <v>772.6793447066512</v>
+      </c>
+      <c r="T39" t="n">
+        <v>-5573.994148843788</v>
+      </c>
+      <c r="U39" t="n">
+        <v>6.051930328543438</v>
+      </c>
+      <c r="V39" t="n">
+        <v>-0.6160297387119786</v>
+      </c>
+      <c r="W39" t="n">
+        <v>4.448162700694659</v>
+      </c>
+      <c r="X39" t="n">
+        <v>7.536013850330467</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>9</v>
+      </c>
+      <c r="C40" t="n">
+        <v>163.5538240585597</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2.29744128560822</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:39.000000000</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>78.16082160591883</v>
+      </c>
+      <c r="G40" t="n">
+        <v>75.15052164927901</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I40" t="n">
+        <v>2685.571758676042</v>
+      </c>
+      <c r="J40" t="n">
+        <v>76.69722857860863</v>
+      </c>
+      <c r="K40" t="n">
+        <v>187.1355458357606</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.07075238307678021</v>
+      </c>
+      <c r="M40" t="n">
+        <v>-18.23506257730739</v>
+      </c>
+      <c r="N40" t="n">
+        <v>46.69722857860863</v>
+      </c>
+      <c r="O40" t="n">
+        <v>30</v>
+      </c>
+      <c r="P40" t="n">
+        <v>-110.438317257152</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>-110.438317257152</v>
+      </c>
+      <c r="R40" t="n">
+        <v>4180.609575994578</v>
+      </c>
+      <c r="S40" t="n">
+        <v>772.0628703534514</v>
+      </c>
+      <c r="T40" t="n">
+        <v>-5569.542845609092</v>
+      </c>
+      <c r="U40" t="n">
+        <v>6.047103583339349</v>
+      </c>
+      <c r="V40" t="n">
+        <v>-0.6169221434443384</v>
+      </c>
+      <c r="W40" t="n">
+        <v>4.454617717555306</v>
+      </c>
+      <c r="X40" t="n">
+        <v>7.536025058893129</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>9</v>
+      </c>
+      <c r="C41" t="n">
+        <v>163.5538240585597</v>
+      </c>
+      <c r="D41" t="n">
+        <v>2.29744128560822</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:39.000000000</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>97.65969775264597</v>
+      </c>
+      <c r="G41" t="n">
+        <v>94.64939779600616</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I41" t="n">
+        <v>2685.571758676042</v>
+      </c>
+      <c r="J41" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K41" t="n">
+        <v>187.1355458357606</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O41" t="n">
+        <v>30</v>
+      </c>
+      <c r="P41" t="n">
+        <v>-90.93944111042482</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>-90.93944111042482</v>
+      </c>
+      <c r="R41" t="n">
+        <v>4180.609575994578</v>
+      </c>
+      <c r="S41" t="n">
+        <v>772.0628703534514</v>
+      </c>
+      <c r="T41" t="n">
+        <v>-5569.542845609092</v>
+      </c>
+      <c r="U41" t="n">
+        <v>6.047103583339349</v>
+      </c>
+      <c r="V41" t="n">
+        <v>-0.6169221434443384</v>
+      </c>
+      <c r="W41" t="n">
+        <v>4.454617717555306</v>
+      </c>
+      <c r="X41" t="n">
+        <v>7.536025058893129</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>9</v>
+      </c>
+      <c r="C42" t="n">
+        <v>163.5307958202829</v>
+      </c>
+      <c r="D42" t="n">
+        <v>2.364564445292875</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:40.000000000</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>77.95746087489442</v>
+      </c>
+      <c r="G42" t="n">
+        <v>74.94716091825461</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I42" t="n">
+        <v>2678.72266758524</v>
+      </c>
+      <c r="J42" t="n">
+        <v>76.47168767739386</v>
+      </c>
+      <c r="K42" t="n">
+        <v>187.1133656655702</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.07095731826867091</v>
+      </c>
+      <c r="M42" t="n">
+        <v>-18.24278907214466</v>
+      </c>
+      <c r="N42" t="n">
+        <v>46.47168767739386</v>
+      </c>
+      <c r="O42" t="n">
+        <v>30</v>
+      </c>
+      <c r="P42" t="n">
+        <v>-110.6416779881764</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>-110.6416779881764</v>
+      </c>
+      <c r="R42" t="n">
+        <v>4186.654134981074</v>
+      </c>
+      <c r="S42" t="n">
+        <v>771.4455039683504</v>
+      </c>
+      <c r="T42" t="n">
+        <v>-5565.085090068063</v>
+      </c>
+      <c r="U42" t="n">
+        <v>6.042269816583015</v>
+      </c>
+      <c r="V42" t="n">
+        <v>-0.6178138418177311</v>
+      </c>
+      <c r="W42" t="n">
+        <v>4.461067620043642</v>
+      </c>
+      <c r="X42" t="n">
+        <v>7.536036278451264</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>9</v>
+      </c>
+      <c r="C43" t="n">
+        <v>163.5307958202829</v>
+      </c>
+      <c r="D43" t="n">
+        <v>2.364564445292875</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:40.000000000</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>97.68187792283635</v>
+      </c>
+      <c r="G43" t="n">
+        <v>94.67157796619654</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I43" t="n">
+        <v>2678.72266758524</v>
+      </c>
+      <c r="J43" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K43" t="n">
+        <v>187.1133656655702</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O43" t="n">
+        <v>30</v>
+      </c>
+      <c r="P43" t="n">
+        <v>-90.91726094023444</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>-90.91726094023444</v>
+      </c>
+      <c r="R43" t="n">
+        <v>4186.654134981074</v>
+      </c>
+      <c r="S43" t="n">
+        <v>771.4455039683504</v>
+      </c>
+      <c r="T43" t="n">
+        <v>-5565.085090068063</v>
+      </c>
+      <c r="U43" t="n">
+        <v>6.042269816583015</v>
+      </c>
+      <c r="V43" t="n">
+        <v>-0.6178138418177311</v>
+      </c>
+      <c r="W43" t="n">
+        <v>4.461067620043642</v>
+      </c>
+      <c r="X43" t="n">
+        <v>7.536036278451264</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>9</v>
+      </c>
+      <c r="C44" t="n">
+        <v>163.5076658118871</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2.431871441127972</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:41.000000000</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>77.74750284355764</v>
+      </c>
+      <c r="G44" t="n">
+        <v>74.73720288691783</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I44" t="n">
+        <v>2671.87410903505</v>
+      </c>
+      <c r="J44" t="n">
+        <v>76.23949442306588</v>
+      </c>
+      <c r="K44" t="n">
+        <v>187.091130442579</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0.07116384019692897</v>
+      </c>
+      <c r="M44" t="n">
+        <v>-18.25054378740238</v>
+      </c>
+      <c r="N44" t="n">
+        <v>46.23949442306588</v>
+      </c>
+      <c r="O44" t="n">
+        <v>30</v>
+      </c>
+      <c r="P44" t="n">
+        <v>-110.8516360195132</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>-110.8516360195132</v>
+      </c>
+      <c r="R44" t="n">
+        <v>4192.693856232201</v>
+      </c>
+      <c r="S44" t="n">
+        <v>770.8272493231128</v>
+      </c>
+      <c r="T44" t="n">
+        <v>-5560.620887318662</v>
+      </c>
+      <c r="U44" t="n">
+        <v>6.037429034159843</v>
+      </c>
+      <c r="V44" t="n">
+        <v>-0.6187048284063847</v>
+      </c>
+      <c r="W44" t="n">
+        <v>4.467512400678472</v>
+      </c>
+      <c r="X44" t="n">
+        <v>7.536047508968182</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>9</v>
+      </c>
+      <c r="C45" t="n">
+        <v>163.5076658118871</v>
+      </c>
+      <c r="D45" t="n">
+        <v>2.431871441127972</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:41.000000000</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>97.70411314582753</v>
+      </c>
+      <c r="G45" t="n">
+        <v>94.69381318918772</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I45" t="n">
+        <v>2671.87410903505</v>
+      </c>
+      <c r="J45" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K45" t="n">
+        <v>187.091130442579</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O45" t="n">
+        <v>30</v>
+      </c>
+      <c r="P45" t="n">
+        <v>-90.89502571724324</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>-90.89502571724324</v>
+      </c>
+      <c r="R45" t="n">
+        <v>4192.693856232201</v>
+      </c>
+      <c r="S45" t="n">
+        <v>770.8272493231128</v>
+      </c>
+      <c r="T45" t="n">
+        <v>-5560.620887318662</v>
+      </c>
+      <c r="U45" t="n">
+        <v>6.037429034159843</v>
+      </c>
+      <c r="V45" t="n">
+        <v>-0.6187048284063847</v>
+      </c>
+      <c r="W45" t="n">
+        <v>4.467512400678472</v>
+      </c>
+      <c r="X45" t="n">
+        <v>7.536047508968182</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>9</v>
+      </c>
+      <c r="C46" t="n">
+        <v>163.4844332917572</v>
+      </c>
+      <c r="D46" t="n">
+        <v>2.499363679460058</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:42.000000000</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>77.53061505113172</v>
+      </c>
+      <c r="G46" t="n">
+        <v>74.52031509449191</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I46" t="n">
+        <v>2665.026093371957</v>
+      </c>
+      <c r="J46" t="n">
+        <v>76.00031611042111</v>
+      </c>
+      <c r="K46" t="n">
+        <v>187.0688399223602</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0.07137193596577533</v>
+      </c>
+      <c r="M46" t="n">
+        <v>-18.2581771768836</v>
+      </c>
+      <c r="N46" t="n">
+        <v>46.00031611042112</v>
+      </c>
+      <c r="O46" t="n">
+        <v>30</v>
+      </c>
+      <c r="P46" t="n">
+        <v>-111.0685238119391</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>-111.0685238119391</v>
+      </c>
+      <c r="R46" t="n">
+        <v>4198.728733844372</v>
+      </c>
+      <c r="S46" t="n">
+        <v>770.2081009969961</v>
+      </c>
+      <c r="T46" t="n">
+        <v>-5556.150242500321</v>
+      </c>
+      <c r="U46" t="n">
+        <v>6.032581240642913</v>
+      </c>
+      <c r="V46" t="n">
+        <v>-0.6195951109660709</v>
+      </c>
+      <c r="W46" t="n">
+        <v>4.473952051944367</v>
+      </c>
+      <c r="X46" t="n">
+        <v>7.536058750407076</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>9</v>
+      </c>
+      <c r="C47" t="n">
+        <v>163.4844332917572</v>
+      </c>
+      <c r="D47" t="n">
+        <v>2.499363679460058</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:42.000000000</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>97.72640366604637</v>
+      </c>
+      <c r="G47" t="n">
+        <v>94.71610370940655</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I47" t="n">
+        <v>2665.026093371957</v>
+      </c>
+      <c r="J47" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K47" t="n">
+        <v>187.0688399223602</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O47" t="n">
+        <v>30</v>
+      </c>
+      <c r="P47" t="n">
+        <v>-90.87273519702441</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>-90.87273519702441</v>
+      </c>
+      <c r="R47" t="n">
+        <v>4198.728733844372</v>
+      </c>
+      <c r="S47" t="n">
+        <v>770.2081009969961</v>
+      </c>
+      <c r="T47" t="n">
+        <v>-5556.150242500321</v>
+      </c>
+      <c r="U47" t="n">
+        <v>6.032581240642913</v>
+      </c>
+      <c r="V47" t="n">
+        <v>-0.6195951109660709</v>
+      </c>
+      <c r="W47" t="n">
+        <v>4.473952051944367</v>
+      </c>
+      <c r="X47" t="n">
+        <v>7.536058750407076</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>9</v>
+      </c>
+      <c r="C48" t="n">
+        <v>163.46109732498</v>
+      </c>
+      <c r="D48" t="n">
+        <v>2.567042547016628</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:43.000000000</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>77.30636889140453</v>
+      </c>
+      <c r="G48" t="n">
+        <v>74.29606893476472</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I48" t="n">
+        <v>2658.178634404458</v>
+      </c>
+      <c r="J48" t="n">
+        <v>75.75372389836676</v>
+      </c>
+      <c r="K48" t="n">
+        <v>187.046493870033</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.07158164979677206</v>
+      </c>
+      <c r="M48" t="n">
+        <v>-18.2658369356172</v>
+      </c>
+      <c r="N48" t="n">
+        <v>45.75372389836676</v>
+      </c>
+      <c r="O48" t="n">
+        <v>30</v>
+      </c>
+      <c r="P48" t="n">
+        <v>-111.2927699716663</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>-111.2927699716663</v>
+      </c>
+      <c r="R48" t="n">
+        <v>4204.758760252277</v>
+      </c>
+      <c r="S48" t="n">
+        <v>769.5880627614288</v>
+      </c>
+      <c r="T48" t="n">
+        <v>-5551.67316074104</v>
+      </c>
+      <c r="U48" t="n">
+        <v>6.027726441949745</v>
+      </c>
+      <c r="V48" t="n">
+        <v>-0.6204846840661218</v>
+      </c>
+      <c r="W48" t="n">
+        <v>4.480386566349355</v>
+      </c>
+      <c r="X48" t="n">
+        <v>7.536070002731167</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>9</v>
+      </c>
+      <c r="C49" t="n">
+        <v>163.46109732498</v>
+      </c>
+      <c r="D49" t="n">
+        <v>2.567042547016628</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:43.000000000</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>97.74874971837355</v>
+      </c>
+      <c r="G49" t="n">
+        <v>94.73844976173373</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I49" t="n">
+        <v>2658.178634404458</v>
+      </c>
+      <c r="J49" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K49" t="n">
+        <v>187.046493870033</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O49" t="n">
+        <v>30</v>
+      </c>
+      <c r="P49" t="n">
+        <v>-90.85038914469726</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>-90.85038914469726</v>
+      </c>
+      <c r="R49" t="n">
+        <v>4204.758760252277</v>
+      </c>
+      <c r="S49" t="n">
+        <v>769.5880627614288</v>
+      </c>
+      <c r="T49" t="n">
+        <v>-5551.67316074104</v>
+      </c>
+      <c r="U49" t="n">
+        <v>6.027726441949745</v>
+      </c>
+      <c r="V49" t="n">
+        <v>-0.6204846840661218</v>
+      </c>
+      <c r="W49" t="n">
+        <v>4.480386566349355</v>
+      </c>
+      <c r="X49" t="n">
+        <v>7.536070002731167</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>9</v>
+      </c>
+      <c r="C50" t="n">
+        <v>163.4376569660906</v>
+      </c>
+      <c r="D50" t="n">
+        <v>2.634909443945261</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:44.000000000</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>77.07433180019035</v>
+      </c>
+      <c r="G50" t="n">
+        <v>74.06403184355054</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I50" t="n">
+        <v>2651.331746062029</v>
+      </c>
+      <c r="J50" t="n">
+        <v>75.49928498656621</v>
+      </c>
+      <c r="K50" t="n">
+        <v>187.0240920494467</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0.0717929979294957</v>
+      </c>
+      <c r="M50" t="n">
+        <v>-18.2735225603786</v>
+      </c>
+      <c r="N50" t="n">
+        <v>45.49928498656621</v>
+      </c>
+      <c r="O50" t="n">
+        <v>30</v>
+      </c>
+      <c r="P50" t="n">
+        <v>-111.5248070628804</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>-111.5248070628804</v>
+      </c>
+      <c r="R50" t="n">
+        <v>4210.783927892788</v>
+      </c>
+      <c r="S50" t="n">
+        <v>768.9671384068922</v>
+      </c>
+      <c r="T50" t="n">
+        <v>-5547.189647180097</v>
+      </c>
+      <c r="U50" t="n">
+        <v>6.022864644012732</v>
+      </c>
+      <c r="V50" t="n">
+        <v>-0.621373542290163</v>
+      </c>
+      <c r="W50" t="n">
+        <v>4.486815936401529</v>
+      </c>
+      <c r="X50" t="n">
+        <v>7.536081265903624</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>9</v>
+      </c>
+      <c r="C51" t="n">
+        <v>163.4376569660906</v>
+      </c>
+      <c r="D51" t="n">
+        <v>2.634909443945261</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>22 Jun 2025 10:15:44.000000000</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>97.7711515389599</v>
+      </c>
+      <c r="G51" t="n">
+        <v>94.76085158232009</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I51" t="n">
+        <v>2651.331746062029</v>
+      </c>
+      <c r="J51" t="n">
+        <v>96.19610472533579</v>
+      </c>
+      <c r="K51" t="n">
+        <v>187.0240920494467</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" t="n">
+        <v>66.19610472533577</v>
+      </c>
+      <c r="O51" t="n">
+        <v>30</v>
+      </c>
+      <c r="P51" t="n">
+        <v>-90.82798732411089</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>-90.82798732411089</v>
+      </c>
+      <c r="R51" t="n">
+        <v>4210.783927892788</v>
+      </c>
+      <c r="S51" t="n">
+        <v>768.9671384068922</v>
+      </c>
+      <c r="T51" t="n">
+        <v>-5547.189647180097</v>
+      </c>
+      <c r="U51" t="n">
+        <v>6.022864644012732</v>
+      </c>
+      <c r="V51" t="n">
+        <v>-0.621373542290163</v>
+      </c>
+      <c r="W51" t="n">
+        <v>4.486815936401529</v>
+      </c>
+      <c r="X51" t="n">
+        <v>7.536081265903624</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>9</v>
+      </c>
+      <c r="C52" t="n">
         <v>163.4141114460597</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D52" t="n">
         <v>2.702965818087287</v>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>22 Jun 2025 10:15:45.000000000</t>
         </is>
       </c>
-      <c r="F27" t="n">
-        <v>-2.57474546176051</v>
-      </c>
-      <c r="G27" t="n">
-        <v>-5.585045418400322</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0.2285989647435062</v>
-      </c>
-      <c r="I27" t="n">
+      <c r="F52" t="n">
+        <v>76.8340675537257</v>
+      </c>
+      <c r="G52" t="n">
+        <v>73.82376759708589</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1e-30</v>
+      </c>
+      <c r="I52" t="n">
         <v>2644.485438987418</v>
       </c>
-      <c r="J27" t="n">
-        <v>-4.172250112854694</v>
-      </c>
-      <c r="K27" t="n">
+      <c r="J52" t="n">
+        <v>75.2365629026315</v>
+      </c>
+      <c r="K52" t="n">
         <v>187.0016342119766</v>
       </c>
-      <c r="L27" t="n">
-        <v>67.20544793794559</v>
-      </c>
-      <c r="M27" t="n">
-        <v>-93.16057254106825</v>
-      </c>
-      <c r="N27" t="n">
-        <v>-34.1722501128547</v>
-      </c>
-      <c r="O27" t="n">
-        <v>30</v>
-      </c>
-      <c r="P27" t="n">
-        <v>-191.1738843248313</v>
-      </c>
-      <c r="Q27" t="n">
-        <v>-191.1738843248313</v>
-      </c>
-      <c r="R27" t="n">
+      <c r="L52" t="n">
+        <v>0.07200596800293901</v>
+      </c>
+      <c r="M52" t="n">
+        <v>-18.28108408934932</v>
+      </c>
+      <c r="N52" t="n">
+        <v>45.23656290263151</v>
+      </c>
+      <c r="O52" t="n">
+        <v>30</v>
+      </c>
+      <c r="P52" t="n">
+        <v>-111.7650713093451</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>-111.7650713093451</v>
+      </c>
+      <c r="R52" t="n">
         <v>4216.804230896475</v>
       </c>
-      <c r="S27" t="n">
+      <c r="S52" t="n">
         <v>768.3453224869243</v>
       </c>
-      <c r="T27" t="n">
+      <c r="T52" t="n">
         <v>-5542.6997069643</v>
       </c>
-      <c r="U27" t="n">
+      <c r="U52" t="n">
         <v>6.017995851409331</v>
       </c>
-      <c r="V27" t="n">
+      <c r="V52" t="n">
         <v>-0.6222616933785181</v>
       </c>
-      <c r="W27" t="n">
+      <c r="W52" t="n">
         <v>4.493240154623779</v>
       </c>
-      <c r="X27" t="n">
+      <c r="X52" t="n">
         <v>7.536092539887614</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix to previous commit
</commit_message>
<xml_diff>
--- a/Reports/EnvBobLog.xlsx
+++ b/Reports/EnvBobLog.xlsx
@@ -579,10 +579,10 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>97.24842937034347</v>
+        <v>32.18686796864258</v>
       </c>
       <c r="G2" t="n">
-        <v>94.23812941370366</v>
+        <v>29.17656801200277</v>
       </c>
       <c r="H2" t="n">
         <v>1e-30</v>
@@ -591,28 +591,28 @@
         <v>2815.78946910655</v>
       </c>
       <c r="J2" t="n">
-        <v>96.19610472533579</v>
+        <v>31.13454332363488</v>
       </c>
       <c r="K2" t="n">
         <v>187.5468142180631</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.9998303855186813</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>-89.70751609533153</v>
       </c>
       <c r="N2" t="n">
-        <v>66.19610472533577</v>
+        <v>1.134543323634884</v>
       </c>
       <c r="O2" t="n">
         <v>30</v>
       </c>
       <c r="P2" t="n">
-        <v>-91.35070949272732</v>
+        <v>-156.4122708944282</v>
       </c>
       <c r="Q2" t="n">
-        <v>-91.35070949272732</v>
+        <v>-156.4122708944282</v>
       </c>
       <c r="R2" t="n">
         <v>4064.853260246761</v>
@@ -636,7 +636,7 @@
         <v>7.535814018149579</v>
       </c>
       <c r="Y2" t="n">
-        <v>163.9731205251298</v>
+        <v>164.9731205251298</v>
       </c>
       <c r="Z2" t="n">
         <v>1.055284896272219</v>
@@ -661,10 +661,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>97.26960680290232</v>
+        <v>32.13272442994204</v>
       </c>
       <c r="G3" t="n">
-        <v>94.2593068462625</v>
+        <v>29.12242447330222</v>
       </c>
       <c r="H3" t="n">
         <v>1e-30</v>
@@ -673,28 +673,28 @@
         <v>2808.932536949855</v>
       </c>
       <c r="J3" t="n">
-        <v>96.19610472533579</v>
+        <v>31.0592223523755</v>
       </c>
       <c r="K3" t="n">
         <v>187.5256367855042</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>0.9998092312782793</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>-89.6893696308077</v>
       </c>
       <c r="N3" t="n">
-        <v>66.19610472533577</v>
+        <v>1.059222352375495</v>
       </c>
       <c r="O3" t="n">
         <v>30</v>
       </c>
       <c r="P3" t="n">
-        <v>-91.32953206016848</v>
+        <v>-156.4664144331288</v>
       </c>
       <c r="Q3" t="n">
-        <v>-91.32953206016848</v>
+        <v>-156.4664144331288</v>
       </c>
       <c r="R3" t="n">
         <v>4070.988386033326</v>
@@ -718,10 +718,10 @@
         <v>7.535825022542807</v>
       </c>
       <c r="Y3" t="n">
-        <v>163.951872253482</v>
+        <v>164.951872253482</v>
       </c>
       <c r="Z3" t="n">
-        <v>1.11916110502662</v>
+        <v>1.119161105026607</v>
       </c>
     </row>
     <row r="4">
@@ -743,10 +743,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>97.29083503050288</v>
+        <v>32.07326550682729</v>
       </c>
       <c r="G4" t="n">
-        <v>94.28053507386306</v>
+        <v>29.06296555018748</v>
       </c>
       <c r="H4" t="n">
         <v>1e-30</v>
@@ -755,28 +755,28 @@
         <v>2802.075916028852</v>
       </c>
       <c r="J4" t="n">
-        <v>96.19610472533579</v>
+        <v>30.97853520166019</v>
       </c>
       <c r="K4" t="n">
         <v>187.5044085579037</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>0.9997867767228594</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>-89.67112636331564</v>
       </c>
       <c r="N4" t="n">
-        <v>66.19610472533577</v>
+        <v>0.9785352016601896</v>
       </c>
       <c r="O4" t="n">
         <v>30</v>
       </c>
       <c r="P4" t="n">
-        <v>-91.30830383256792</v>
+        <v>-156.5258733562435</v>
       </c>
       <c r="Q4" t="n">
-        <v>-91.30830383256792</v>
+        <v>-156.5258733562435</v>
       </c>
       <c r="R4" t="n">
         <v>4077.118808914962</v>
@@ -800,7 +800,7 @@
         <v>7.535836038587997</v>
       </c>
       <c r="Y4" t="n">
-        <v>163.9305370533707</v>
+        <v>164.9305370533707</v>
       </c>
       <c r="Z4" t="n">
         <v>1.183197228970331</v>
@@ -825,10 +825,10 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>97.31211426277841</v>
+        <v>32.00830851785484</v>
       </c>
       <c r="G5" t="n">
-        <v>94.3018143061386</v>
+        <v>28.99800856121502</v>
       </c>
       <c r="H5" t="n">
         <v>1e-30</v>
@@ -837,28 +837,28 @@
         <v>2795.219618218265</v>
       </c>
       <c r="J5" t="n">
-        <v>96.19610472533579</v>
+        <v>30.8922989804122</v>
       </c>
       <c r="K5" t="n">
         <v>187.4831293256281</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>0.9997630120876797</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>-89.65278546701178</v>
       </c>
       <c r="N5" t="n">
-        <v>66.19610472533577</v>
+        <v>0.8922989804121995</v>
       </c>
       <c r="O5" t="n">
         <v>30</v>
       </c>
       <c r="P5" t="n">
-        <v>-91.28702460029238</v>
+        <v>-156.5908303452159</v>
       </c>
       <c r="Q5" t="n">
-        <v>-91.28702460029238</v>
+        <v>-156.5908303452159</v>
       </c>
       <c r="R5" t="n">
         <v>4083.244521195483</v>
@@ -882,7 +882,7 @@
         <v>7.535847066248904</v>
       </c>
       <c r="Y5" t="n">
-        <v>163.9091141611784</v>
+        <v>164.9091141611784</v>
       </c>
       <c r="Z5" t="n">
         <v>1.247394412869355</v>
@@ -907,10 +907,10 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>97.33344472090315</v>
+        <v>31.9376552141014</v>
       </c>
       <c r="G6" t="n">
-        <v>94.32314476426333</v>
+        <v>28.92735525746158</v>
       </c>
       <c r="H6" t="n">
         <v>1e-30</v>
@@ -919,28 +919,28 @@
         <v>2788.363652149048</v>
       </c>
       <c r="J6" t="n">
-        <v>96.19610472533579</v>
+        <v>30.80031521853403</v>
       </c>
       <c r="K6" t="n">
         <v>187.4617988675034</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>0.9997379274823645</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>-89.63434610152402</v>
       </c>
       <c r="N6" t="n">
-        <v>66.19610472533577</v>
+        <v>0.8003152185340365</v>
       </c>
       <c r="O6" t="n">
         <v>30</v>
       </c>
       <c r="P6" t="n">
-        <v>-91.26569414216766</v>
+        <v>-156.6614836489694</v>
       </c>
       <c r="Q6" t="n">
-        <v>-91.26569414216766</v>
+        <v>-156.6614836489694</v>
       </c>
       <c r="R6" t="n">
         <v>4089.365516921297</v>
@@ -964,10 +964,10 @@
         <v>7.535858105489311</v>
       </c>
       <c r="Y6" t="n">
-        <v>163.8876029772208</v>
+        <v>164.8876029772208</v>
       </c>
       <c r="Z6" t="n">
-        <v>1.311753843689576</v>
+        <v>1.311753843689601</v>
       </c>
     </row>
     <row r="7">
@@ -989,10 +989,10 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>97.35482661695511</v>
+        <v>31.86109041358749</v>
       </c>
       <c r="G7" t="n">
-        <v>94.3445266603153</v>
+        <v>28.85079045694768</v>
       </c>
       <c r="H7" t="n">
         <v>1e-30</v>
@@ -1001,28 +1001,28 @@
         <v>2781.50802986114</v>
       </c>
       <c r="J7" t="n">
-        <v>96.19610472533579</v>
+        <v>30.70236852196818</v>
       </c>
       <c r="K7" t="n">
         <v>187.4404169714515</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>0.9997115129086226</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>-89.61580742140809</v>
       </c>
       <c r="N7" t="n">
-        <v>66.19610472533577</v>
+        <v>0.7023685219681762</v>
       </c>
       <c r="O7" t="n">
         <v>30</v>
       </c>
       <c r="P7" t="n">
-        <v>-91.2443122461157</v>
+        <v>-156.7380484494833</v>
       </c>
       <c r="Q7" t="n">
-        <v>-91.2443122461157</v>
+        <v>-156.7380484494833</v>
       </c>
       <c r="R7" t="n">
         <v>4095.481788411548</v>
@@ -1046,7 +1046,7 @@
         <v>7.535869156272923</v>
       </c>
       <c r="Y7" t="n">
-        <v>163.8660027232646</v>
+        <v>164.8660027232646</v>
       </c>
       <c r="Z7" t="n">
         <v>1.376276688121171</v>
@@ -1071,10 +1071,10 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>97.37626016760281</v>
+        <v>31.77838036939573</v>
       </c>
       <c r="G8" t="n">
-        <v>94.365960210963</v>
+        <v>28.76808041275592</v>
       </c>
       <c r="H8" t="n">
         <v>1e-30</v>
@@ -1083,28 +1083,28 @@
         <v>2774.652762393974</v>
       </c>
       <c r="J8" t="n">
-        <v>96.19610472533579</v>
+        <v>30.5982249271287</v>
       </c>
       <c r="K8" t="n">
         <v>187.4189834208038</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>0.9996837582455187</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>-89.59716856961302</v>
       </c>
       <c r="N8" t="n">
-        <v>66.19610472533577</v>
+        <v>0.5982249271286952</v>
       </c>
       <c r="O8" t="n">
         <v>30</v>
       </c>
       <c r="P8" t="n">
-        <v>-91.22287869546797</v>
+        <v>-156.820758493675</v>
       </c>
       <c r="Q8" t="n">
-        <v>-91.22287869546797</v>
+        <v>-156.820758493675</v>
       </c>
       <c r="R8" t="n">
         <v>4101.593328551306</v>
@@ -1128,10 +1128,10 @@
         <v>7.535880218563409</v>
       </c>
       <c r="Y8" t="n">
-        <v>163.844312670568</v>
+        <v>164.844312670568</v>
       </c>
       <c r="Z8" t="n">
-        <v>1.440964134184441</v>
+        <v>1.440964134184429</v>
       </c>
     </row>
     <row r="9">
@@ -1153,10 +1153,10 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>97.39774558737386</v>
+        <v>31.68927098393819</v>
       </c>
       <c r="G9" t="n">
-        <v>94.38744563073405</v>
+        <v>28.67897102729838</v>
       </c>
       <c r="H9" t="n">
         <v>1e-30</v>
@@ -1165,28 +1165,28 @@
         <v>2767.797861948103</v>
       </c>
       <c r="J9" t="n">
-        <v>96.19610472533579</v>
+        <v>30.4876301219001</v>
       </c>
       <c r="K9" t="n">
         <v>187.3974980010327</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>0.9996546532558847</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>-89.57842868012946</v>
       </c>
       <c r="N9" t="n">
-        <v>66.19610472533577</v>
+        <v>0.4876301219001064</v>
       </c>
       <c r="O9" t="n">
         <v>30</v>
       </c>
       <c r="P9" t="n">
-        <v>-91.20139327569692</v>
+        <v>-156.9098678791326</v>
       </c>
       <c r="Q9" t="n">
-        <v>-91.20139327569692</v>
+        <v>-156.9098678791326</v>
       </c>
       <c r="R9" t="n">
         <v>4107.700129693329</v>
@@ -1210,7 +1210,7 @@
         <v>7.535891292324466</v>
       </c>
       <c r="Y9" t="n">
-        <v>163.8225320244808</v>
+        <v>164.8225320244808</v>
       </c>
       <c r="Z9" t="n">
         <v>1.505817370914526</v>
@@ -1235,10 +1235,10 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>97.41928310241255</v>
+        <v>31.59348568897201</v>
       </c>
       <c r="G10" t="n">
-        <v>94.40898314577274</v>
+        <v>28.5831857323322</v>
       </c>
       <c r="H10" t="n">
         <v>1e-30</v>
@@ -1247,28 +1247,28 @@
         <v>2760.943337502153</v>
       </c>
       <c r="J10" t="n">
-        <v>96.19610472533579</v>
+        <v>30.37030731189524</v>
       </c>
       <c r="K10" t="n">
         <v>187.375960485994</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.9996241875635582</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>-89.55958687265007</v>
       </c>
       <c r="N10" t="n">
-        <v>66.19610472533577</v>
+        <v>0.3703073118952399</v>
       </c>
       <c r="O10" t="n">
         <v>30</v>
       </c>
       <c r="P10" t="n">
-        <v>-91.17985576065823</v>
+        <v>-157.0056531740988</v>
       </c>
       <c r="Q10" t="n">
-        <v>-91.17985576065823</v>
+        <v>-157.0056531740988</v>
       </c>
       <c r="R10" t="n">
         <v>4113.802185896458</v>
@@ -1292,7 +1292,7 @@
         <v>7.535902377519727</v>
       </c>
       <c r="Y10" t="n">
-        <v>163.8006601567133</v>
+        <v>164.8006601567133</v>
       </c>
       <c r="Z10" t="n">
         <v>1.570837630214003</v>
@@ -1317,10 +1317,10 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>97.4408729295702</v>
+        <v>31.49072321436286</v>
       </c>
       <c r="G11" t="n">
-        <v>94.43057297293039</v>
+        <v>28.48042325772305</v>
       </c>
       <c r="H11" t="n">
         <v>1e-30</v>
@@ -1329,28 +1329,28 @@
         <v>2754.089201487097</v>
       </c>
       <c r="J11" t="n">
-        <v>96.19610472533579</v>
+        <v>30.24595501012843</v>
       </c>
       <c r="K11" t="n">
         <v>187.3543706588364</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.9995923506849465</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>-89.54064226057424</v>
       </c>
       <c r="N11" t="n">
-        <v>66.19610472533577</v>
+        <v>0.2459550101284312</v>
       </c>
       <c r="O11" t="n">
         <v>30</v>
       </c>
       <c r="P11" t="n">
-        <v>-91.15826593350057</v>
+        <v>-157.1084156487079</v>
       </c>
       <c r="Q11" t="n">
-        <v>-91.15826593350057</v>
+        <v>-157.1084156487079</v>
       </c>
       <c r="R11" t="n">
         <v>4119.899489477398</v>
@@ -1374,10 +1374,10 @@
         <v>7.53591347411274</v>
       </c>
       <c r="Y11" t="n">
-        <v>163.778696257454</v>
+        <v>164.778696257454</v>
       </c>
       <c r="Z11" t="n">
-        <v>1.636026123521763</v>
+        <v>1.636026123521776</v>
       </c>
     </row>
     <row r="12">
@@ -1399,10 +1399,10 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>97.4625152870881</v>
+        <v>31.38065485199084</v>
       </c>
       <c r="G12" t="n">
-        <v>94.45221533044828</v>
+        <v>28.37035489535102</v>
       </c>
       <c r="H12" t="n">
         <v>1e-30</v>
@@ -1411,28 +1411,28 @@
         <v>2747.235466369206</v>
       </c>
       <c r="J12" t="n">
-        <v>96.19610472533579</v>
+        <v>30.11424429023853</v>
       </c>
       <c r="K12" t="n">
         <v>187.3327283013185</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>0.9995591320062571</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>-89.52159394625795</v>
       </c>
       <c r="N12" t="n">
-        <v>66.19610472533577</v>
+        <v>0.1142442902385287</v>
       </c>
       <c r="O12" t="n">
         <v>30</v>
       </c>
       <c r="P12" t="n">
-        <v>-91.13662357598271</v>
+        <v>-157.2184840110799</v>
       </c>
       <c r="Q12" t="n">
-        <v>-91.13662357598271</v>
+        <v>-157.2184840110799</v>
       </c>
       <c r="R12" t="n">
         <v>4125.992032816553</v>
@@ -1456,7 +1456,7 @@
         <v>7.535924582067136</v>
       </c>
       <c r="Y12" t="n">
-        <v>163.75663950775</v>
+        <v>164.75663950775</v>
       </c>
       <c r="Z12" t="n">
         <v>1.70138407432339</v>
@@ -1481,10 +1481,10 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>97.4842104048922</v>
+        <v>31.26292138114069</v>
       </c>
       <c r="G13" t="n">
-        <v>94.47391044825238</v>
+        <v>28.25262142450088</v>
       </c>
       <c r="H13" t="n">
         <v>1e-30</v>
@@ -1493,28 +1493,28 @@
         <v>2740.382141405968</v>
       </c>
       <c r="J13" t="n">
-        <v>96.19610472533579</v>
+        <v>29.97481570158428</v>
       </c>
       <c r="K13" t="n">
         <v>187.3110331835144</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>0.9995245207745809</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>-89.50244101794314</v>
       </c>
       <c r="N13" t="n">
-        <v>66.19610472533577</v>
+        <v>-0.02518429841572235</v>
       </c>
       <c r="O13" t="n">
         <v>30</v>
       </c>
       <c r="P13" t="n">
-        <v>-91.11492845817861</v>
+        <v>-157.3362174819301</v>
       </c>
       <c r="Q13" t="n">
-        <v>-91.11492845817861</v>
+        <v>-157.3362174819301</v>
       </c>
       <c r="R13" t="n">
         <v>4132.079809975929</v>
@@ -1538,10 +1538,10 @@
         <v>7.535935701346451</v>
       </c>
       <c r="Y13" t="n">
-        <v>163.7344892568628</v>
+        <v>164.7344892568628</v>
       </c>
       <c r="Z13" t="n">
-        <v>1.766912749526267</v>
+        <v>1.76691274952628</v>
       </c>
     </row>
     <row r="14">
@@ -1563,10 +1563,10 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>97.50595850360671</v>
+        <v>31.13712962278723</v>
       </c>
       <c r="G14" t="n">
-        <v>94.49565854696689</v>
+        <v>28.12682966614742</v>
       </c>
       <c r="H14" t="n">
         <v>1e-30</v>
@@ -1575,28 +1575,28 @@
         <v>2733.529239295291</v>
       </c>
       <c r="J14" t="n">
-        <v>96.19610472533579</v>
+        <v>29.8272758445163</v>
       </c>
       <c r="K14" t="n">
         <v>187.2892850847998</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>0.9994885061177748</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>-89.48318255647936</v>
       </c>
       <c r="N14" t="n">
-        <v>66.19610472533577</v>
+        <v>-0.1727241554837027</v>
       </c>
       <c r="O14" t="n">
         <v>30</v>
       </c>
       <c r="P14" t="n">
-        <v>-91.09318035946407</v>
+        <v>-157.4620092402835</v>
       </c>
       <c r="Q14" t="n">
-        <v>-91.09318035946407</v>
+        <v>-157.4620092402835</v>
       </c>
       <c r="R14" t="n">
         <v>4138.162813305039</v>
@@ -1620,10 +1620,10 @@
         <v>7.535946831914168</v>
       </c>
       <c r="Y14" t="n">
-        <v>163.7122446700199</v>
+        <v>164.7122446700199</v>
       </c>
       <c r="Z14" t="n">
-        <v>1.832613395866888</v>
+        <v>1.832613395866875</v>
       </c>
     </row>
     <row r="15">
@@ -1645,10 +1645,10 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>97.52775980873048</v>
+        <v>31.00284835529074</v>
       </c>
       <c r="G15" t="n">
-        <v>94.51745985209067</v>
+        <v>27.99254839865093</v>
       </c>
       <c r="H15" t="n">
         <v>1e-30</v>
@@ -1657,28 +1657,28 @@
         <v>2726.676771686951</v>
       </c>
       <c r="J15" t="n">
-        <v>96.19610472533579</v>
+        <v>29.67119327189604</v>
       </c>
       <c r="K15" t="n">
         <v>187.2674837796761</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>0.9994510770300681</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>-89.46381763035788</v>
       </c>
       <c r="N15" t="n">
-        <v>66.19610472533577</v>
+        <v>-0.3288067281039592</v>
       </c>
       <c r="O15" t="n">
         <v>30</v>
       </c>
       <c r="P15" t="n">
-        <v>-91.0713790543403</v>
+        <v>-157.5962905077801</v>
       </c>
       <c r="Q15" t="n">
-        <v>-91.0713790543403</v>
+        <v>-157.5962905077801</v>
       </c>
       <c r="R15" t="n">
         <v>4144.241035757347</v>
@@ -1702,10 +1702,10 @@
         <v>7.535957973733796</v>
       </c>
       <c r="Y15" t="n">
-        <v>163.6899049626078</v>
+        <v>164.6899049626078</v>
       </c>
       <c r="Z15" t="n">
-        <v>1.8984872830552</v>
+        <v>1.898487283055213</v>
       </c>
     </row>
     <row r="16">
@@ -1727,10 +1727,10 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>97.54961454338027</v>
+        <v>30.85960364338833</v>
       </c>
       <c r="G16" t="n">
-        <v>94.53931458674046</v>
+        <v>27.84930368674851</v>
       </c>
       <c r="H16" t="n">
         <v>1e-30</v>
@@ -1739,28 +1739,28 @@
         <v>2719.824751472531</v>
       </c>
       <c r="J16" t="n">
-        <v>96.19610472533579</v>
+        <v>29.50609382534384</v>
       </c>
       <c r="K16" t="n">
         <v>187.2456290450263</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>0.999412222376258</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>-89.44434529775604</v>
       </c>
       <c r="N16" t="n">
-        <v>66.19610472533577</v>
+        <v>-0.493906174656159</v>
       </c>
       <c r="O16" t="n">
         <v>30</v>
       </c>
       <c r="P16" t="n">
-        <v>-91.04952431969053</v>
+        <v>-157.7395352196825</v>
       </c>
       <c r="Q16" t="n">
-        <v>-91.04952431969053</v>
+        <v>-157.7395352196825</v>
       </c>
       <c r="R16" t="n">
         <v>4150.314469700492</v>
@@ -1784,10 +1784,10 @@
         <v>7.535969126768791</v>
       </c>
       <c r="Y16" t="n">
-        <v>163.6674692819926</v>
+        <v>164.6674692819926</v>
       </c>
       <c r="Z16" t="n">
-        <v>1.964535681859003</v>
+        <v>1.964535681859015</v>
       </c>
     </row>
     <row r="17">
@@ -1809,10 +1809,10 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>97.5715229426915</v>
+        <v>30.70687330176955</v>
       </c>
       <c r="G17" t="n">
-        <v>94.56122298605169</v>
+        <v>27.69657334512974</v>
       </c>
       <c r="H17" t="n">
         <v>1e-30</v>
@@ -1821,28 +1821,28 @@
         <v>2712.973188276437</v>
       </c>
       <c r="J17" t="n">
-        <v>96.19610472533579</v>
+        <v>29.33145508441383</v>
       </c>
       <c r="K17" t="n">
         <v>187.223720645715</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>0.9993719308670929</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>-89.42476460275672</v>
       </c>
       <c r="N17" t="n">
-        <v>66.19610472533577</v>
+        <v>-0.6685449155861717</v>
       </c>
       <c r="O17" t="n">
         <v>30</v>
       </c>
       <c r="P17" t="n">
-        <v>-91.02761592037929</v>
+        <v>-157.8922655613012</v>
       </c>
       <c r="Q17" t="n">
-        <v>-91.02761592037929</v>
+        <v>-157.8922655613012</v>
       </c>
       <c r="R17" t="n">
         <v>4156.383109219659</v>
@@ -1866,10 +1866,10 @@
         <v>7.535980290982569</v>
       </c>
       <c r="Y17" t="n">
-        <v>163.6449369459386</v>
+        <v>164.6449369459386</v>
       </c>
       <c r="Z17" t="n">
-        <v>2.030759907970641</v>
+        <v>2.030759907970616</v>
       </c>
     </row>
     <row r="18">
@@ -1891,10 +1891,10 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>97.59348523238316</v>
+        <v>30.54408065727787</v>
       </c>
       <c r="G18" t="n">
-        <v>94.58318527574335</v>
+        <v>27.53378070063806</v>
       </c>
       <c r="H18" t="n">
         <v>1e-30</v>
@@ -1903,28 +1903,28 @@
         <v>2706.122095179903</v>
       </c>
       <c r="J18" t="n">
-        <v>96.19610472533579</v>
+        <v>29.14670015023048</v>
       </c>
       <c r="K18" t="n">
         <v>187.2017583560234</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>0.9993301910937288</v>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
+        <v>-89.40507458061377</v>
       </c>
       <c r="N18" t="n">
-        <v>66.19610472533577</v>
+        <v>-0.853299849769517</v>
       </c>
       <c r="O18" t="n">
         <v>30</v>
       </c>
       <c r="P18" t="n">
-        <v>-91.00565363068762</v>
+        <v>-158.0550582057929</v>
       </c>
       <c r="Q18" t="n">
-        <v>-91.00565363068762</v>
+        <v>-158.0550582057929</v>
       </c>
       <c r="R18" t="n">
         <v>4162.446946698016</v>
@@ -1948,10 +1948,10 @@
         <v>7.535991466338523</v>
       </c>
       <c r="Y18" t="n">
-        <v>163.6223070849084</v>
+        <v>164.6223070849084</v>
       </c>
       <c r="Z18" t="n">
-        <v>2.097161257011621</v>
+        <v>2.097161257011583</v>
       </c>
     </row>
     <row r="19">
@@ -1973,10 +1973,10 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>97.61550163947105</v>
+        <v>30.37058701374187</v>
       </c>
       <c r="G19" t="n">
-        <v>94.60520168283124</v>
+        <v>27.36028705710206</v>
       </c>
       <c r="H19" t="n">
         <v>1e-30</v>
@@ -1985,28 +1985,28 @@
         <v>2699.271485352876</v>
       </c>
       <c r="J19" t="n">
-        <v>96.19610472533579</v>
+        <v>28.95119009960661</v>
       </c>
       <c r="K19" t="n">
         <v>187.1797419489355</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>0.9992869915093044</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>-89.38527425452611</v>
       </c>
       <c r="N19" t="n">
-        <v>66.19610472533577</v>
+        <v>-1.048809900393394</v>
       </c>
       <c r="O19" t="n">
         <v>30</v>
       </c>
       <c r="P19" t="n">
-        <v>-90.98363722359976</v>
+        <v>-158.2285518493289</v>
       </c>
       <c r="Q19" t="n">
-        <v>-90.98363722359976</v>
+        <v>-158.2285518493289</v>
       </c>
       <c r="R19" t="n">
         <v>4168.505974541447</v>
@@ -2030,10 +2030,10 @@
         <v>7.536002652800055</v>
       </c>
       <c r="Y19" t="n">
-        <v>163.5995788196273</v>
+        <v>164.5995788196273</v>
       </c>
       <c r="Z19" t="n">
-        <v>2.163741037189362</v>
+        <v>2.16374103718935</v>
       </c>
     </row>
     <row r="20">
@@ -2055,10 +2055,10 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>97.63757240298672</v>
+        <v>30.18568272886018</v>
       </c>
       <c r="G20" t="n">
-        <v>94.62727244634691</v>
+        <v>27.17538277222037</v>
       </c>
       <c r="H20" t="n">
         <v>1e-30</v>
@@ -2067,28 +2067,28 @@
         <v>2692.421368734845</v>
       </c>
       <c r="J20" t="n">
-        <v>96.19610472533579</v>
+        <v>28.74421505120923</v>
       </c>
       <c r="K20" t="n">
         <v>187.1576711854198</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>0.9992423204035747</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>-89.36536263381332</v>
       </c>
       <c r="N20" t="n">
-        <v>66.19610472533577</v>
+        <v>-1.255784948790768</v>
       </c>
       <c r="O20" t="n">
         <v>30</v>
       </c>
       <c r="P20" t="n">
-        <v>-90.96156646008407</v>
+        <v>-158.4134561342106</v>
       </c>
       <c r="Q20" t="n">
-        <v>-90.96156646008407</v>
+        <v>-158.4134561342106</v>
       </c>
       <c r="R20" t="n">
         <v>4174.560186828104</v>
@@ -2112,10 +2112,10 @@
         <v>7.536013850330467</v>
       </c>
       <c r="Y20" t="n">
-        <v>163.5767514431665</v>
+        <v>164.5767514431665</v>
       </c>
       <c r="Z20" t="n">
-        <v>2.230500602020816</v>
+        <v>2.230500602020829</v>
       </c>
     </row>
     <row r="21">
@@ -2137,10 +2137,10 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>97.65969775264597</v>
+        <v>29.9885769074284</v>
       </c>
       <c r="G21" t="n">
-        <v>94.64939779600616</v>
+        <v>26.97827695078858</v>
       </c>
       <c r="H21" t="n">
         <v>1e-30</v>
@@ -2149,28 +2149,28 @@
         <v>2685.571758676042</v>
       </c>
       <c r="J21" t="n">
-        <v>96.19610472533579</v>
+        <v>28.5249838801182</v>
       </c>
       <c r="K21" t="n">
         <v>187.1355458357606</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>0.9991961659424652</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>-89.34533871766905</v>
       </c>
       <c r="N21" t="n">
-        <v>66.19610472533577</v>
+        <v>-1.4750161198818</v>
       </c>
       <c r="O21" t="n">
         <v>30</v>
       </c>
       <c r="P21" t="n">
-        <v>-90.93944111042482</v>
+        <v>-158.6105619556424</v>
       </c>
       <c r="Q21" t="n">
-        <v>-90.93944111042482</v>
+        <v>-158.6105619556424</v>
       </c>
       <c r="R21" t="n">
         <v>4180.609575994578</v>
@@ -2194,10 +2194,10 @@
         <v>7.536025058893129</v>
       </c>
       <c r="Y21" t="n">
-        <v>163.5538240585597</v>
+        <v>164.5538240585597</v>
       </c>
       <c r="Z21" t="n">
-        <v>2.297441285608205</v>
+        <v>2.297441285608218</v>
       </c>
     </row>
     <row r="22">
@@ -2219,10 +2219,10 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>97.68187792283635</v>
+        <v>29.7783848018303</v>
       </c>
       <c r="G22" t="n">
-        <v>94.67157796619654</v>
+        <v>26.76808484519049</v>
       </c>
       <c r="H22" t="n">
         <v>1e-30</v>
@@ -2231,28 +2231,28 @@
         <v>2678.72266758524</v>
       </c>
       <c r="J22" t="n">
-        <v>96.19610472533579</v>
+        <v>28.29261160432972</v>
       </c>
       <c r="K22" t="n">
         <v>187.1133656655702</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>0.9991485161412397</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>-89.32520149252396</v>
       </c>
       <c r="N22" t="n">
-        <v>66.19610472533577</v>
+        <v>-1.707388395670275</v>
       </c>
       <c r="O22" t="n">
         <v>30</v>
       </c>
       <c r="P22" t="n">
-        <v>-90.91726094023444</v>
+        <v>-158.8207540612405</v>
       </c>
       <c r="Q22" t="n">
-        <v>-90.91726094023444</v>
+        <v>-158.8207540612405</v>
       </c>
       <c r="R22" t="n">
         <v>4186.654134981074</v>
@@ -2276,10 +2276,10 @@
         <v>7.536036278451264</v>
       </c>
       <c r="Y22" t="n">
-        <v>163.5307958202829</v>
+        <v>164.5307958202829</v>
       </c>
       <c r="Z22" t="n">
-        <v>2.364564445292857</v>
+        <v>2.364564445292896</v>
       </c>
     </row>
     <row r="23">
@@ -2301,10 +2301,10 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>97.70411314582753</v>
+        <v>29.55411283394943</v>
       </c>
       <c r="G23" t="n">
-        <v>94.69381318918772</v>
+        <v>26.54381287730961</v>
       </c>
       <c r="H23" t="n">
         <v>1e-30</v>
@@ -2313,28 +2313,28 @@
         <v>2671.87410903505</v>
       </c>
       <c r="J23" t="n">
-        <v>96.19610472533579</v>
+        <v>28.04610441345766</v>
       </c>
       <c r="K23" t="n">
         <v>187.091130442579</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>0.9990993588730406</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>-89.3049499325263</v>
       </c>
       <c r="N23" t="n">
-        <v>66.19610472533577</v>
+        <v>-1.953895586542343</v>
       </c>
       <c r="O23" t="n">
         <v>30</v>
       </c>
       <c r="P23" t="n">
-        <v>-90.89502571724324</v>
+        <v>-159.0450260291214</v>
       </c>
       <c r="Q23" t="n">
-        <v>-90.89502571724324</v>
+        <v>-159.0450260291214</v>
       </c>
       <c r="R23" t="n">
         <v>4192.693856232201</v>
@@ -2358,7 +2358,7 @@
         <v>7.536047508968182</v>
       </c>
       <c r="Y23" t="n">
-        <v>163.5076658118871</v>
+        <v>164.5076658118871</v>
       </c>
       <c r="Z23" t="n">
         <v>2.431871441127968</v>
@@ -2383,10 +2383,10 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>97.72640366604637</v>
+        <v>29.3146402853062</v>
       </c>
       <c r="G24" t="n">
-        <v>94.71610370940655</v>
+        <v>26.30434032866638</v>
       </c>
       <c r="H24" t="n">
         <v>1e-30</v>
@@ -2395,28 +2395,28 @@
         <v>2665.026093371957</v>
       </c>
       <c r="J24" t="n">
-        <v>96.19610472533579</v>
+        <v>27.7843413445956</v>
       </c>
       <c r="K24" t="n">
         <v>187.0688399223602</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>0.9990486818376649</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>-89.28458299814335</v>
       </c>
       <c r="N24" t="n">
-        <v>66.19610472533577</v>
+        <v>-2.215658655404402</v>
       </c>
       <c r="O24" t="n">
         <v>30</v>
       </c>
       <c r="P24" t="n">
-        <v>-90.87273519702441</v>
+        <v>-159.2844985777646</v>
       </c>
       <c r="Q24" t="n">
-        <v>-90.87273519702441</v>
+        <v>-159.2844985777646</v>
       </c>
       <c r="R24" t="n">
         <v>4198.728733844372</v>
@@ -2440,7 +2440,7 @@
         <v>7.536058750407076</v>
       </c>
       <c r="Y24" t="n">
-        <v>163.4844332917572</v>
+        <v>164.4844332917572</v>
       </c>
       <c r="Z24" t="n">
         <v>2.499363679460075</v>
@@ -2465,10 +2465,10 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>97.74874971837355</v>
+        <v>29.05869735166444</v>
       </c>
       <c r="G25" t="n">
-        <v>94.73844976173373</v>
+        <v>26.04839739502463</v>
       </c>
       <c r="H25" t="n">
         <v>1e-30</v>
@@ -2477,28 +2477,28 @@
         <v>2658.178634404458</v>
       </c>
       <c r="J25" t="n">
-        <v>96.19610472533579</v>
+        <v>27.50605235862668</v>
       </c>
       <c r="K25" t="n">
         <v>187.046493870033</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>0.9989964726062094</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>-89.26409963822117</v>
       </c>
       <c r="N25" t="n">
-        <v>66.19610472533577</v>
+        <v>-2.493947641373323</v>
       </c>
       <c r="O25" t="n">
         <v>30</v>
       </c>
       <c r="P25" t="n">
-        <v>-90.85038914469726</v>
+        <v>-159.5404415114064</v>
       </c>
       <c r="Q25" t="n">
-        <v>-90.85038914469726</v>
+        <v>-159.5404415114064</v>
       </c>
       <c r="R25" t="n">
         <v>4204.758760252277</v>
@@ -2522,7 +2522,7 @@
         <v>7.536070002731167</v>
       </c>
       <c r="Y25" t="n">
-        <v>163.46109732498</v>
+        <v>164.46109732498</v>
       </c>
       <c r="Z25" t="n">
         <v>2.567042547016642</v>
@@ -2547,10 +2547,10 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>97.7711515389599</v>
+        <v>28.78483781347484</v>
       </c>
       <c r="G26" t="n">
-        <v>94.76085158232009</v>
+        <v>25.77453785683503</v>
       </c>
       <c r="H26" t="n">
         <v>1e-30</v>
@@ -2559,28 +2559,28 @@
         <v>2651.331746062029</v>
       </c>
       <c r="J26" t="n">
-        <v>96.19610472533579</v>
+        <v>27.20979099985072</v>
       </c>
       <c r="K26" t="n">
         <v>187.0240920494467</v>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>0.9989427185964026</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>-89.24349878833677</v>
       </c>
       <c r="N26" t="n">
-        <v>66.19610472533577</v>
+        <v>-2.79020900014928</v>
       </c>
       <c r="O26" t="n">
         <v>30</v>
       </c>
       <c r="P26" t="n">
-        <v>-90.82798732411089</v>
+        <v>-159.8143010495959</v>
       </c>
       <c r="Q26" t="n">
-        <v>-90.82798732411089</v>
+        <v>-159.8143010495959</v>
       </c>
       <c r="R26" t="n">
         <v>4210.783927892788</v>
@@ -2604,10 +2604,10 @@
         <v>7.536081265903624</v>
       </c>
       <c r="Y26" t="n">
-        <v>163.4376569660906</v>
+        <v>164.4376569660906</v>
       </c>
       <c r="Z26" t="n">
-        <v>2.634909443945255</v>
+        <v>2.63490944394523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>